<commit_message>
Graph for Eviction times
</commit_message>
<xml_diff>
--- a/tests/pfbenchmark/test_results/data.xlsx
+++ b/tests/pfbenchmark/test_results/data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,46 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcfadden8/umap/src/umap/tests/pfbenchmark/test_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{404CCEA0-2457-694B-B9D2-CAA4B942EE1E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235CA318-F790-E34F-99BD-44E9E393F48F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="50700" windowHeight="31540"/>
+    <workbookView xWindow="-51200" yWindow="-820" windowWidth="51200" windowHeight="31540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">data!$C$23:$C$31</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">data!$K$16:$K$22</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">data!$C$23:$C$31</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">data!$K$16:$K$22</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">data!$K$23:$K$31</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">data!$K$32:$K$38</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">data!$K$39:$K$47</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">data!$C$23:$C$31</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">data!$K$16:$K$22</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">data!$K$23:$K$31</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">data!$K$32:$K$38</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">data!$K$39:$K$47</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">data!$K$23:$K$31</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">data!$C$23:$C$31</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">data!$K$16:$K$22</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">data!$K$23:$K$31</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">data!$K$32:$K$38</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">data!$K$39:$K$47</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">data!$K$32:$K$38</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">data!$K$39:$K$47</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">data!$C$23:$C$31</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">data!$K$16:$K$22</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">data!$K$23:$K$31</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">data!$K$32:$K$38</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">data!$K$39:$K$47</definedName>
-  </definedNames>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="22">
   <si>
     <t>test</t>
   </si>
@@ -102,11 +75,23 @@
   <si>
     <t>store MiB/s</t>
   </si>
+  <si>
+    <t>80 UFFD Threads - Clean Evictions</t>
+  </si>
+  <si>
+    <t>80 UFFD Threads - Dirty Evictions</t>
+  </si>
+  <si>
+    <t>1 UFFD Thread - Clean Evictions</t>
+  </si>
+  <si>
+    <t>1 UFFD Thread - Dirty Evictions</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1436,7 +1421,867 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>UMAP Eviction Bandwidth</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>(4k</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Page Eviction)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$A$56</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>80 UFFD Threads - Clean Evictions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$C$27:$C$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$F$27:$F$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3457</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3559</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3501</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3623</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3655</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3617</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4052</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3950</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3912</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FE4D-894B-8B12-F2A4039BC474}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$A$57</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>80 UFFD Threads - Dirty Evictions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$C$27:$C$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$F$45:$F$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>28768</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28978</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29506</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29600</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29639</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29529</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29552</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>31713</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33733</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FE4D-894B-8B12-F2A4039BC474}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$A$58</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1 UFFD Thread - Clean Evictions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$C$27:$C$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$F$18:$F$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>709</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>754</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>759</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>756</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>734</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>748</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FE4D-894B-8B12-F2A4039BC474}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$A$59</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1 UFFD Thread - Dirty Evictions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$C$27:$C$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$F$36:$F$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>5923</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5717</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6195</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6476</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6744</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6399</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6520</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6767</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6924</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-FE4D-894B-8B12-F2A4039BC474}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1342641007"/>
+        <c:axId val="1441500303"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1342641007"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>OMP Threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1441500303"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1441500303"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>IOPS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1342641007"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1992,6 +2837,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2025,6 +3386,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>30235</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>43846</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F3F5F96-995C-A942-94A7-05EBA14725CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2329,11 +3728,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="R51" sqref="R51"/>
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2412,27 +3811,27 @@
         <v>171</v>
       </c>
       <c r="I2" s="2">
-        <f>1000000000/E2</f>
+        <f t="shared" ref="I2:I33" si="0">1000000000/E2</f>
         <v>207641.19601328904</v>
       </c>
       <c r="J2" s="2">
-        <f>1000000000/G2</f>
+        <f t="shared" ref="J2:J33" si="1">1000000000/G2</f>
         <v>548245.61403508775</v>
       </c>
       <c r="K2" s="2">
-        <f>1000000000/H2</f>
+        <f t="shared" ref="K2:K33" si="2">1000000000/H2</f>
         <v>5847953.2163742688</v>
       </c>
       <c r="L2" s="2">
-        <f>I2*4096/(1024*1024)</f>
+        <f t="shared" ref="L2:L33" si="3">I2*4096/(1024*1024)</f>
         <v>811.09842192691031</v>
       </c>
       <c r="M2" s="2">
-        <f>J2*4096/(1024*1024)</f>
+        <f t="shared" ref="M2:M33" si="4">J2*4096/(1024*1024)</f>
         <v>2141.5844298245615</v>
       </c>
       <c r="N2" s="2">
-        <f>K2*4096/(1024*1024)</f>
+        <f t="shared" ref="N2:N33" si="5">K2*4096/(1024*1024)</f>
         <v>22843.567251461987</v>
       </c>
     </row>
@@ -2462,27 +3861,27 @@
         <v>1872</v>
       </c>
       <c r="I3" s="2">
-        <f>1000000000/E3</f>
+        <f t="shared" si="0"/>
         <v>252525.25252525252</v>
       </c>
       <c r="J3" s="2">
-        <f>1000000000/G3</f>
+        <f t="shared" si="1"/>
         <v>345542.50172771252</v>
       </c>
       <c r="K3" s="2">
-        <f>1000000000/H3</f>
+        <f t="shared" si="2"/>
         <v>534188.03418803425</v>
       </c>
       <c r="L3" s="2">
-        <f>I3*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>986.42676767676767</v>
       </c>
       <c r="M3" s="2">
-        <f>J3*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>1349.775397373877</v>
       </c>
       <c r="N3" s="2">
-        <f>K3*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>2086.6720085470088</v>
       </c>
     </row>
@@ -2512,27 +3911,27 @@
         <v>224</v>
       </c>
       <c r="I4" s="2">
-        <f>1000000000/E4</f>
+        <f t="shared" si="0"/>
         <v>192418.70309794112</v>
       </c>
       <c r="J4" s="2">
-        <f>1000000000/G4</f>
+        <f t="shared" si="1"/>
         <v>314366.55139893113</v>
       </c>
       <c r="K4" s="2">
-        <f>1000000000/H4</f>
+        <f t="shared" si="2"/>
         <v>4464285.7142857146</v>
       </c>
       <c r="L4" s="2">
-        <f>I4*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>751.6355589763325</v>
       </c>
       <c r="M4" s="2">
-        <f>J4*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>1227.9943414020747</v>
       </c>
       <c r="N4" s="2">
-        <f>K4*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>17438.616071428572</v>
       </c>
     </row>
@@ -2562,27 +3961,27 @@
         <v>90</v>
       </c>
       <c r="I5" s="2">
-        <f>1000000000/E5</f>
+        <f t="shared" si="0"/>
         <v>212134.06873143828</v>
       </c>
       <c r="J5" s="2">
-        <f>1000000000/G5</f>
+        <f t="shared" si="1"/>
         <v>307881.77339901478</v>
       </c>
       <c r="K5" s="2">
-        <f>1000000000/H5</f>
+        <f t="shared" si="2"/>
         <v>11111111.111111112</v>
       </c>
       <c r="L5" s="2">
-        <f>I5*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>828.64870598218079</v>
       </c>
       <c r="M5" s="2">
-        <f>J5*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>1202.6631773399015</v>
       </c>
       <c r="N5" s="2">
-        <f>K5*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>43402.777777777781</v>
       </c>
     </row>
@@ -2612,27 +4011,27 @@
         <v>402</v>
       </c>
       <c r="I6" s="2">
-        <f>1000000000/E6</f>
+        <f t="shared" si="0"/>
         <v>136817.62210972773</v>
       </c>
       <c r="J6" s="2">
-        <f>1000000000/G6</f>
+        <f t="shared" si="1"/>
         <v>361271.67630057805</v>
       </c>
       <c r="K6" s="2">
-        <f>1000000000/H6</f>
+        <f t="shared" si="2"/>
         <v>2487562.1890547262</v>
       </c>
       <c r="L6" s="2">
-        <f>I6*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>534.44383636612395</v>
       </c>
       <c r="M6" s="2">
-        <f>J6*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>1411.217485549133</v>
       </c>
       <c r="N6" s="2">
-        <f>K6*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>9717.0398009950241</v>
       </c>
     </row>
@@ -2662,27 +4061,27 @@
         <v>845</v>
       </c>
       <c r="I7" s="2">
-        <f>1000000000/E7</f>
+        <f t="shared" si="0"/>
         <v>131700.25023047545</v>
       </c>
       <c r="J7" s="2">
-        <f>1000000000/G7</f>
+        <f t="shared" si="1"/>
         <v>351493.848857645</v>
       </c>
       <c r="K7" s="2">
-        <f>1000000000/H7</f>
+        <f t="shared" si="2"/>
         <v>1183431.952662722</v>
       </c>
       <c r="L7" s="2">
-        <f>I7*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>514.45410246279471</v>
       </c>
       <c r="M7" s="2">
-        <f>J7*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>1373.0228471001758</v>
       </c>
       <c r="N7" s="2">
-        <f>K7*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>4622.7810650887577</v>
       </c>
     </row>
@@ -2712,27 +4111,27 @@
         <v>421</v>
       </c>
       <c r="I8" s="2">
-        <f>1000000000/E8</f>
+        <f t="shared" si="0"/>
         <v>102732.6895418122</v>
       </c>
       <c r="J8" s="2">
-        <f>1000000000/G8</f>
+        <f t="shared" si="1"/>
         <v>483792.93662312528</v>
       </c>
       <c r="K8" s="2">
-        <f>1000000000/H8</f>
+        <f t="shared" si="2"/>
         <v>2375296.9121140144</v>
       </c>
       <c r="L8" s="2">
-        <f>I8*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>401.29956852270391</v>
       </c>
       <c r="M8" s="2">
-        <f>J8*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>1889.8161586840831</v>
       </c>
       <c r="N8" s="2">
-        <f>K8*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>9278.5035629453687</v>
       </c>
     </row>
@@ -2762,27 +4161,27 @@
         <v>670</v>
       </c>
       <c r="I9" s="2">
-        <f>1000000000/E9</f>
+        <f t="shared" si="0"/>
         <v>69720.421111343516</v>
       </c>
       <c r="J9" s="2">
-        <f>1000000000/G9</f>
+        <f t="shared" si="1"/>
         <v>325520.83333333331</v>
       </c>
       <c r="K9" s="2">
-        <f>1000000000/H9</f>
+        <f t="shared" si="2"/>
         <v>1492537.3134328357</v>
       </c>
       <c r="L9" s="2">
-        <f>I9*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>272.34539496618561</v>
       </c>
       <c r="M9" s="2">
-        <f>J9*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>1271.5657552083333</v>
       </c>
       <c r="N9" s="2">
-        <f>K9*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>5830.2238805970146</v>
       </c>
     </row>
@@ -2812,27 +4211,27 @@
         <v>609</v>
       </c>
       <c r="I10" s="2">
-        <f>1000000000/E10</f>
+        <f t="shared" si="0"/>
         <v>20168.202811447471</v>
       </c>
       <c r="J10" s="2">
-        <f>1000000000/G10</f>
+        <f t="shared" si="1"/>
         <v>434404.86533449177</v>
       </c>
       <c r="K10" s="2">
-        <f>1000000000/H10</f>
+        <f t="shared" si="2"/>
         <v>1642036.1247947456</v>
       </c>
       <c r="L10" s="2">
-        <f>I10*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>78.782042232216682</v>
       </c>
       <c r="M10" s="2">
-        <f>J10*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>1696.8940052128585</v>
       </c>
       <c r="N10" s="2">
-        <f>K10*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>6414.2036124794749</v>
       </c>
     </row>
@@ -2862,27 +4261,27 @@
         <v>904</v>
       </c>
       <c r="I11" s="2">
-        <f>1000000000/E11</f>
+        <f t="shared" si="0"/>
         <v>19346.101760495261</v>
       </c>
       <c r="J11" s="2">
-        <f>1000000000/G11</f>
+        <f t="shared" si="1"/>
         <v>329163.92363396974</v>
       </c>
       <c r="K11" s="2">
-        <f>1000000000/H11</f>
+        <f t="shared" si="2"/>
         <v>1106194.6902654867</v>
       </c>
       <c r="L11" s="2">
-        <f>I11*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>75.570710001934614</v>
       </c>
       <c r="M11" s="2">
-        <f>J11*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>1285.7965766951943</v>
       </c>
       <c r="N11" s="2">
-        <f>K11*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>4321.0730088495575</v>
       </c>
     </row>
@@ -2912,27 +4311,27 @@
         <v>1082</v>
       </c>
       <c r="I12" s="2">
-        <f>1000000000/E12</f>
+        <f t="shared" si="0"/>
         <v>14849.573817231445</v>
       </c>
       <c r="J12" s="2">
-        <f>1000000000/G12</f>
+        <f t="shared" si="1"/>
         <v>386697.60247486463</v>
       </c>
       <c r="K12" s="2">
-        <f>1000000000/H12</f>
+        <f t="shared" si="2"/>
         <v>924214.41774491686</v>
       </c>
       <c r="L12" s="2">
-        <f>I12*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>58.006147723560332</v>
       </c>
       <c r="M12" s="2">
-        <f>J12*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>1510.53750966744</v>
       </c>
       <c r="N12" s="2">
-        <f>K12*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>3610.2125693160815</v>
       </c>
     </row>
@@ -2962,27 +4361,27 @@
         <v>1070</v>
       </c>
       <c r="I13" s="2">
-        <f>1000000000/E13</f>
+        <f t="shared" si="0"/>
         <v>14731.879787860931</v>
       </c>
       <c r="J13" s="2">
-        <f>1000000000/G13</f>
+        <f t="shared" si="1"/>
         <v>293858.36027034972</v>
       </c>
       <c r="K13" s="2">
-        <f>1000000000/H13</f>
+        <f t="shared" si="2"/>
         <v>934579.43925233639</v>
       </c>
       <c r="L13" s="2">
-        <f>I13*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>57.546405421331762</v>
       </c>
       <c r="M13" s="2">
-        <f>J13*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>1147.8842198060536</v>
       </c>
       <c r="N13" s="2">
-        <f>K13*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>3650.700934579439</v>
       </c>
     </row>
@@ -3012,27 +4411,27 @@
         <v>528</v>
       </c>
       <c r="I14" s="2">
-        <f>1000000000/E14</f>
+        <f t="shared" si="0"/>
         <v>14430.430892666454</v>
       </c>
       <c r="J14" s="2">
-        <f>1000000000/G14</f>
+        <f t="shared" si="1"/>
         <v>367376.92872887582</v>
       </c>
       <c r="K14" s="2">
-        <f>1000000000/H14</f>
+        <f t="shared" si="2"/>
         <v>1893939.393939394</v>
       </c>
       <c r="L14" s="2">
-        <f>I14*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>56.368870674478337</v>
       </c>
       <c r="M14" s="2">
-        <f>J14*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>1435.0661278471712</v>
       </c>
       <c r="N14" s="2">
-        <f>K14*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>7398.200757575758</v>
       </c>
     </row>
@@ -3062,27 +4461,27 @@
         <v>615</v>
       </c>
       <c r="I15" s="2">
-        <f>1000000000/E15</f>
+        <f t="shared" si="0"/>
         <v>14462.780035578438</v>
       </c>
       <c r="J15" s="2">
-        <f>1000000000/G15</f>
+        <f t="shared" si="1"/>
         <v>311623.55874104082</v>
       </c>
       <c r="K15" s="2">
-        <f>1000000000/H15</f>
+        <f t="shared" si="2"/>
         <v>1626016.2601626017</v>
       </c>
       <c r="L15" s="2">
-        <f>I15*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>56.495234513978275</v>
       </c>
       <c r="M15" s="2">
-        <f>J15*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>1217.2795263321907</v>
       </c>
       <c r="N15" s="2">
-        <f>K15*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>6351.6260162601629</v>
       </c>
     </row>
@@ -3112,27 +4511,27 @@
         <v>679</v>
       </c>
       <c r="I16" s="2">
-        <f>1000000000/E16</f>
+        <f t="shared" si="0"/>
         <v>14541.858740384196</v>
       </c>
       <c r="J16" s="2">
-        <f>1000000000/G16</f>
+        <f t="shared" si="1"/>
         <v>305157.15593530668</v>
       </c>
       <c r="K16" s="2">
-        <f>1000000000/H16</f>
+        <f t="shared" si="2"/>
         <v>1472754.0500736376</v>
       </c>
       <c r="L16" s="2">
-        <f>I16*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>56.804135704625764</v>
       </c>
       <c r="M16" s="2">
-        <f>J16*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>1192.0201403722917</v>
       </c>
       <c r="N16" s="2">
-        <f>K16*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>5752.945508100147</v>
       </c>
     </row>
@@ -3162,27 +4561,27 @@
         <v>1061</v>
       </c>
       <c r="I17" s="2">
-        <f>1000000000/E17</f>
+        <f t="shared" si="0"/>
         <v>14759.7118904239</v>
       </c>
       <c r="J17" s="2">
-        <f>1000000000/G17</f>
+        <f t="shared" si="1"/>
         <v>311915.15907673113</v>
       </c>
       <c r="K17" s="2">
-        <f>1000000000/H17</f>
+        <f t="shared" si="2"/>
         <v>942507.06880301598</v>
       </c>
       <c r="L17" s="2">
-        <f>I17*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>57.655124571968358</v>
       </c>
       <c r="M17" s="2">
-        <f>J17*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>1218.418590143481</v>
       </c>
       <c r="N17" s="2">
-        <f>K17*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>3681.6682375117812</v>
       </c>
     </row>
@@ -3212,27 +4611,27 @@
         <v>18597</v>
       </c>
       <c r="I18" s="2">
-        <f>1000000000/E18</f>
+        <f t="shared" si="0"/>
         <v>47132.016778997975</v>
       </c>
       <c r="J18" s="2">
-        <f>1000000000/G18</f>
+        <f t="shared" si="1"/>
         <v>46110.57315442431</v>
       </c>
       <c r="K18" s="2">
-        <f>1000000000/H18</f>
+        <f t="shared" si="2"/>
         <v>53772.113781792759</v>
       </c>
       <c r="L18" s="2">
-        <f>I18*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>184.10944054296084</v>
       </c>
       <c r="M18" s="2">
-        <f>J18*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>180.11942638446996</v>
       </c>
       <c r="N18" s="2">
-        <f>K18*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>210.04731946012797</v>
       </c>
     </row>
@@ -3262,27 +4661,27 @@
         <v>13537</v>
       </c>
       <c r="I19" s="2">
-        <f>1000000000/E19</f>
+        <f t="shared" si="0"/>
         <v>66916.48822269807</v>
       </c>
       <c r="J19" s="2">
-        <f>1000000000/G19</f>
+        <f t="shared" si="1"/>
         <v>73605.181804799053</v>
       </c>
       <c r="K19" s="2">
-        <f>1000000000/H19</f>
+        <f t="shared" si="2"/>
         <v>73871.611139838962</v>
       </c>
       <c r="L19" s="2">
-        <f>I19*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>261.39253211991434</v>
       </c>
       <c r="M19" s="2">
-        <f>J19*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>287.5202414249963</v>
       </c>
       <c r="N19" s="2">
-        <f>K19*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>288.56098101499595</v>
       </c>
     </row>
@@ -3312,27 +4711,27 @@
         <v>14943</v>
       </c>
       <c r="I20" s="2">
-        <f>1000000000/E20</f>
+        <f t="shared" si="0"/>
         <v>60562.015503875969</v>
       </c>
       <c r="J20" s="2">
-        <f>1000000000/G20</f>
+        <f t="shared" si="1"/>
         <v>53070.105609510159</v>
       </c>
       <c r="K20" s="2">
-        <f>1000000000/H20</f>
+        <f t="shared" si="2"/>
         <v>66920.966338753933</v>
       </c>
       <c r="L20" s="2">
-        <f>I20*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>236.57037306201551</v>
       </c>
       <c r="M20" s="2">
-        <f>J20*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>207.30510003714906</v>
       </c>
       <c r="N20" s="2">
-        <f>K20*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>261.41002476075755</v>
       </c>
     </row>
@@ -3362,27 +4761,27 @@
         <v>13427</v>
       </c>
       <c r="I21" s="2">
-        <f>1000000000/E21</f>
+        <f t="shared" si="0"/>
         <v>59651.634454784064</v>
       </c>
       <c r="J21" s="2">
-        <f>1000000000/G21</f>
+        <f t="shared" si="1"/>
         <v>56401.579244218839</v>
       </c>
       <c r="K21" s="2">
-        <f>1000000000/H21</f>
+        <f t="shared" si="2"/>
         <v>74476.800476651522</v>
       </c>
       <c r="L21" s="2">
-        <f>I21*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>233.01419708900025</v>
       </c>
       <c r="M21" s="2">
-        <f>J21*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>220.31866892272984</v>
       </c>
       <c r="N21" s="2">
-        <f>K21*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>290.92500186192001</v>
       </c>
     </row>
@@ -3412,27 +4811,27 @@
         <v>14138</v>
       </c>
       <c r="I22" s="2">
-        <f>1000000000/E22</f>
+        <f t="shared" si="0"/>
         <v>56666.85555618519</v>
       </c>
       <c r="J22" s="2">
-        <f>1000000000/G22</f>
+        <f t="shared" si="1"/>
         <v>53516.00128438403</v>
       </c>
       <c r="K22" s="2">
-        <f>1000000000/H22</f>
+        <f t="shared" si="2"/>
         <v>70731.362286037634</v>
       </c>
       <c r="L22" s="2">
-        <f>I22*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>221.3549045163484</v>
       </c>
       <c r="M22" s="2">
-        <f>J22*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>209.04688001712512</v>
       </c>
       <c r="N22" s="2">
-        <f>K22*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>276.29438392983451</v>
       </c>
     </row>
@@ -3462,27 +4861,27 @@
         <v>14359</v>
       </c>
       <c r="I23" s="2">
-        <f>1000000000/E23</f>
+        <f t="shared" si="0"/>
         <v>55456.965394853592</v>
       </c>
       <c r="J23" s="2">
-        <f>1000000000/G23</f>
+        <f t="shared" si="1"/>
         <v>52648.204696219858</v>
       </c>
       <c r="K23" s="2">
-        <f>1000000000/H23</f>
+        <f t="shared" si="2"/>
         <v>69642.732780834325</v>
       </c>
       <c r="L23" s="2">
-        <f>I23*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>216.62877107364685</v>
       </c>
       <c r="M23" s="2">
-        <f>J23*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>205.65704959460882</v>
       </c>
       <c r="N23" s="2">
-        <f>K23*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>272.04192492513408</v>
       </c>
     </row>
@@ -3512,27 +4911,27 @@
         <v>15598</v>
       </c>
       <c r="I24" s="2">
-        <f>1000000000/E24</f>
+        <f t="shared" si="0"/>
         <v>48100.048100048101</v>
       </c>
       <c r="J24" s="2">
-        <f>1000000000/G24</f>
+        <f t="shared" si="1"/>
         <v>45687.134502923975</v>
       </c>
       <c r="K24" s="2">
-        <f>1000000000/H24</f>
+        <f t="shared" si="2"/>
         <v>64110.783433773562</v>
       </c>
       <c r="L24" s="2">
-        <f>I24*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>187.8908128908129</v>
       </c>
       <c r="M24" s="2">
-        <f>J24*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>178.46536915204678</v>
       </c>
       <c r="N24" s="2">
-        <f>K24*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>250.43274778817798</v>
       </c>
     </row>
@@ -3562,27 +4961,27 @@
         <v>17959</v>
       </c>
       <c r="I25" s="2">
-        <f>1000000000/E25</f>
+        <f t="shared" si="0"/>
         <v>41330.853482124403</v>
       </c>
       <c r="J25" s="2">
-        <f>1000000000/G25</f>
+        <f t="shared" si="1"/>
         <v>38095.238095238092</v>
       </c>
       <c r="K25" s="2">
-        <f>1000000000/H25</f>
+        <f t="shared" si="2"/>
         <v>55682.387660782893</v>
       </c>
       <c r="L25" s="2">
-        <f>I25*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>161.44864641454845</v>
       </c>
       <c r="M25" s="2">
-        <f>J25*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>148.8095238095238</v>
       </c>
       <c r="N25" s="2">
-        <f>K25*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>217.50932679993318</v>
       </c>
     </row>
@@ -3612,27 +5011,27 @@
         <v>22948</v>
       </c>
       <c r="I26" s="2">
-        <f>1000000000/E26</f>
+        <f t="shared" si="0"/>
         <v>30027.324865627721</v>
       </c>
       <c r="J26" s="2">
-        <f>1000000000/G26</f>
+        <f t="shared" si="1"/>
         <v>29143.473319150176</v>
       </c>
       <c r="K26" s="2">
-        <f>1000000000/H26</f>
+        <f t="shared" si="2"/>
         <v>43576.782290395677</v>
       </c>
       <c r="L26" s="2">
-        <f>I26*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>117.29423775635829</v>
       </c>
       <c r="M26" s="2">
-        <f>J26*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>113.84169265293038</v>
       </c>
       <c r="N26" s="2">
-        <f>K26*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>170.22180582185811</v>
       </c>
     </row>
@@ -3662,27 +5061,27 @@
         <v>19723</v>
       </c>
       <c r="I27" s="2">
-        <f>1000000000/E27</f>
+        <f t="shared" si="0"/>
         <v>46315.594460654902</v>
       </c>
       <c r="J27" s="2">
-        <f>1000000000/G27</f>
+        <f t="shared" si="1"/>
         <v>24551.324543959148</v>
       </c>
       <c r="K27" s="2">
-        <f>1000000000/H27</f>
+        <f t="shared" si="2"/>
         <v>50702.225827713839</v>
       </c>
       <c r="L27" s="2">
-        <f>I27*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>180.92029086193321</v>
       </c>
       <c r="M27" s="2">
-        <f>J27*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>95.903611499840423</v>
       </c>
       <c r="N27" s="2">
-        <f>K27*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>198.05556963950718</v>
       </c>
     </row>
@@ -3712,27 +5111,27 @@
         <v>11303</v>
       </c>
       <c r="I28" s="2">
-        <f>1000000000/E28</f>
+        <f t="shared" si="0"/>
         <v>85623.769158318348</v>
       </c>
       <c r="J28" s="2">
-        <f>1000000000/G28</f>
+        <f t="shared" si="1"/>
         <v>37335.722819593786</v>
       </c>
       <c r="K28" s="2">
-        <f>1000000000/H28</f>
+        <f t="shared" si="2"/>
         <v>88472.087056533666</v>
       </c>
       <c r="L28" s="2">
-        <f>I28*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>334.46784827468105</v>
       </c>
       <c r="M28" s="2">
-        <f>J28*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>145.84266726403823</v>
       </c>
       <c r="N28" s="2">
-        <f>K28*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>345.59409006458463</v>
       </c>
     </row>
@@ -3762,27 +5161,27 @@
         <v>6505</v>
       </c>
       <c r="I29" s="2">
-        <f>1000000000/E29</f>
+        <f t="shared" si="0"/>
         <v>148964.69536719797</v>
       </c>
       <c r="J29" s="2">
-        <f>1000000000/G29</f>
+        <f t="shared" si="1"/>
         <v>53619.302949061661</v>
       </c>
       <c r="K29" s="2">
-        <f>1000000000/H29</f>
+        <f t="shared" si="2"/>
         <v>153727.90161414296</v>
       </c>
       <c r="L29" s="2">
-        <f>I29*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>581.89334127811708</v>
       </c>
       <c r="M29" s="2">
-        <f>J29*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>209.45040214477211</v>
       </c>
       <c r="N29" s="2">
-        <f>K29*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>600.49961568024594</v>
       </c>
     </row>
@@ -3812,27 +5211,27 @@
         <v>5266</v>
       </c>
       <c r="I30" s="2">
-        <f>1000000000/E30</f>
+        <f t="shared" si="0"/>
         <v>173701.58068438421</v>
       </c>
       <c r="J30" s="2">
-        <f>1000000000/G30</f>
+        <f t="shared" si="1"/>
         <v>77736.318407960192</v>
       </c>
       <c r="K30" s="2">
-        <f>1000000000/H30</f>
+        <f t="shared" si="2"/>
         <v>189897.45537409798</v>
       </c>
       <c r="L30" s="2">
-        <f>I30*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>678.52179954837584</v>
       </c>
       <c r="M30" s="2">
-        <f>J30*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>303.6574937810945</v>
       </c>
       <c r="N30" s="2">
-        <f>K30*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>741.78693505507022</v>
       </c>
     </row>
@@ -3862,27 +5261,27 @@
         <v>5956</v>
       </c>
       <c r="I31" s="2">
-        <f>1000000000/E31</f>
+        <f t="shared" si="0"/>
         <v>154297.17636167258</v>
       </c>
       <c r="J31" s="2">
-        <f>1000000000/G31</f>
+        <f t="shared" si="1"/>
         <v>89405.453732677692</v>
       </c>
       <c r="K31" s="2">
-        <f>1000000000/H31</f>
+        <f t="shared" si="2"/>
         <v>167897.91806581599</v>
       </c>
       <c r="L31" s="2">
-        <f>I31*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>602.72334516278352</v>
       </c>
       <c r="M31" s="2">
-        <f>J31*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>349.24005364327223</v>
       </c>
       <c r="N31" s="2">
-        <f>K31*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>655.85124244459371</v>
       </c>
     </row>
@@ -3912,27 +5311,27 @@
         <v>5796</v>
       </c>
       <c r="I32" s="2">
-        <f>1000000000/E32</f>
+        <f t="shared" si="0"/>
         <v>150761.34479119553</v>
       </c>
       <c r="J32" s="2">
-        <f>1000000000/G32</f>
+        <f t="shared" si="1"/>
         <v>96983.803704781298</v>
       </c>
       <c r="K32" s="2">
-        <f>1000000000/H32</f>
+        <f t="shared" si="2"/>
         <v>172532.78122843339</v>
       </c>
       <c r="L32" s="2">
-        <f>I32*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>588.91150309060754</v>
       </c>
       <c r="M32" s="2">
-        <f>J32*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>378.84298322180194</v>
       </c>
       <c r="N32" s="2">
-        <f>K32*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>673.95617667356794</v>
       </c>
     </row>
@@ -3962,27 +5361,27 @@
         <v>4951</v>
       </c>
       <c r="I33" s="2">
-        <f>1000000000/E33</f>
+        <f t="shared" si="0"/>
         <v>140745.95355383534</v>
       </c>
       <c r="J33" s="2">
-        <f>1000000000/G33</f>
+        <f t="shared" si="1"/>
         <v>109158.38882218099</v>
       </c>
       <c r="K33" s="2">
-        <f>1000000000/H33</f>
+        <f t="shared" si="2"/>
         <v>201979.39810139366</v>
       </c>
       <c r="L33" s="2">
-        <f>I33*4096/(1024*1024)</f>
+        <f t="shared" si="3"/>
         <v>549.78888106966929</v>
       </c>
       <c r="M33" s="2">
-        <f>J33*4096/(1024*1024)</f>
+        <f t="shared" si="4"/>
         <v>426.39995633664449</v>
       </c>
       <c r="N33" s="2">
-        <f>K33*4096/(1024*1024)</f>
+        <f t="shared" si="5"/>
         <v>788.98202383356897</v>
       </c>
     </row>
@@ -4012,27 +5411,27 @@
         <v>4324</v>
       </c>
       <c r="I34" s="2">
-        <f>1000000000/E34</f>
+        <f t="shared" ref="I34:I53" si="6">1000000000/E34</f>
         <v>142045.45454545456</v>
       </c>
       <c r="J34" s="2">
-        <f>1000000000/G34</f>
+        <f t="shared" ref="J34:J53" si="7">1000000000/G34</f>
         <v>151883.35358444715</v>
       </c>
       <c r="K34" s="2">
-        <f>1000000000/H34</f>
+        <f t="shared" ref="K34:K53" si="8">1000000000/H34</f>
         <v>231267.34505087882</v>
       </c>
       <c r="L34" s="2">
-        <f>I34*4096/(1024*1024)</f>
+        <f t="shared" ref="L34:L53" si="9">I34*4096/(1024*1024)</f>
         <v>554.86505681818187</v>
       </c>
       <c r="M34" s="2">
-        <f>J34*4096/(1024*1024)</f>
+        <f t="shared" ref="M34:M53" si="10">J34*4096/(1024*1024)</f>
         <v>593.29434993924667</v>
       </c>
       <c r="N34" s="2">
-        <f>K34*4096/(1024*1024)</f>
+        <f t="shared" ref="N34:N53" si="11">K34*4096/(1024*1024)</f>
         <v>903.3880666049954</v>
       </c>
     </row>
@@ -4062,27 +5461,27 @@
         <v>4184</v>
       </c>
       <c r="I35" s="2">
-        <f>1000000000/E35</f>
+        <f t="shared" si="6"/>
         <v>133725.5950788981</v>
       </c>
       <c r="J35" s="2">
-        <f>1000000000/G35</f>
+        <f t="shared" si="7"/>
         <v>129971.40629061607</v>
       </c>
       <c r="K35" s="2">
-        <f>1000000000/H35</f>
+        <f t="shared" si="8"/>
         <v>239005.73613766729</v>
       </c>
       <c r="L35" s="2">
-        <f>I35*4096/(1024*1024)</f>
+        <f t="shared" si="9"/>
         <v>522.3656057769457</v>
       </c>
       <c r="M35" s="2">
-        <f>J35*4096/(1024*1024)</f>
+        <f t="shared" si="10"/>
         <v>507.70080582271902</v>
       </c>
       <c r="N35" s="2">
-        <f>K35*4096/(1024*1024)</f>
+        <f t="shared" si="11"/>
         <v>933.61615678776286</v>
       </c>
     </row>
@@ -4112,27 +5511,27 @@
         <v>43161</v>
       </c>
       <c r="I36" s="2">
-        <f>1000000000/E36</f>
+        <f t="shared" si="6"/>
         <v>18482.921780275025</v>
       </c>
       <c r="J36" s="2">
-        <f>1000000000/G36</f>
+        <f t="shared" si="7"/>
         <v>15420.200462606013</v>
       </c>
       <c r="K36" s="2">
-        <f>1000000000/H36</f>
+        <f t="shared" si="8"/>
         <v>23169.064664859481</v>
       </c>
       <c r="L36" s="2">
-        <f>I36*4096/(1024*1024)</f>
+        <f t="shared" si="9"/>
         <v>72.198913204199314</v>
       </c>
       <c r="M36" s="2">
-        <f>J36*4096/(1024*1024)</f>
+        <f t="shared" si="10"/>
         <v>60.23515805705474</v>
       </c>
       <c r="N36" s="2">
-        <f>K36*4096/(1024*1024)</f>
+        <f t="shared" si="11"/>
         <v>90.504158847107348</v>
       </c>
     </row>
@@ -4162,27 +5561,27 @@
         <v>135403</v>
       </c>
       <c r="I37" s="2">
-        <f>1000000000/E37</f>
+        <f t="shared" si="6"/>
         <v>18589.088205223532</v>
       </c>
       <c r="J37" s="2">
-        <f>1000000000/G37</f>
+        <f t="shared" si="7"/>
         <v>5974.5365253290474</v>
       </c>
       <c r="K37" s="2">
-        <f>1000000000/H37</f>
+        <f t="shared" si="8"/>
         <v>7385.3607379452451</v>
       </c>
       <c r="L37" s="2">
-        <f>I37*4096/(1024*1024)</f>
+        <f t="shared" si="9"/>
         <v>72.613625801654422</v>
       </c>
       <c r="M37" s="2">
-        <f>J37*4096/(1024*1024)</f>
+        <f t="shared" si="10"/>
         <v>23.338033302066592</v>
       </c>
       <c r="N37" s="2">
-        <f>K37*4096/(1024*1024)</f>
+        <f t="shared" si="11"/>
         <v>28.849065382598614</v>
       </c>
     </row>
@@ -4212,27 +5611,27 @@
         <v>141203</v>
       </c>
       <c r="I38" s="2">
-        <f>1000000000/E38</f>
+        <f t="shared" si="6"/>
         <v>20085.564504790407</v>
       </c>
       <c r="J38" s="2">
-        <f>1000000000/G38</f>
+        <f t="shared" si="7"/>
         <v>4940.8091068993463</v>
       </c>
       <c r="K38" s="2">
-        <f>1000000000/H38</f>
+        <f t="shared" si="8"/>
         <v>7082.0025070288875</v>
       </c>
       <c r="L38" s="2">
-        <f>I38*4096/(1024*1024)</f>
+        <f t="shared" si="9"/>
         <v>78.459236346837528</v>
       </c>
       <c r="M38" s="2">
-        <f>J38*4096/(1024*1024)</f>
+        <f t="shared" si="10"/>
         <v>19.300035573825571</v>
       </c>
       <c r="N38" s="2">
-        <f>K38*4096/(1024*1024)</f>
+        <f t="shared" si="11"/>
         <v>27.664072293081592</v>
       </c>
     </row>
@@ -4262,27 +5661,27 @@
         <v>163299</v>
       </c>
       <c r="I39" s="2">
-        <f>1000000000/E39</f>
+        <f t="shared" si="6"/>
         <v>20568.090664143649</v>
       </c>
       <c r="J39" s="2">
-        <f>1000000000/G39</f>
+        <f t="shared" si="7"/>
         <v>3931.9149605432335</v>
       </c>
       <c r="K39" s="2">
-        <f>1000000000/H39</f>
+        <f t="shared" si="8"/>
         <v>6123.7362139388488</v>
       </c>
       <c r="L39" s="2">
-        <f>I39*4096/(1024*1024)</f>
+        <f t="shared" si="9"/>
         <v>80.344104156811127</v>
       </c>
       <c r="M39" s="2">
-        <f>J39*4096/(1024*1024)</f>
+        <f t="shared" si="10"/>
         <v>15.359042814622006</v>
       </c>
       <c r="N39" s="2">
-        <f>K39*4096/(1024*1024)</f>
+        <f t="shared" si="11"/>
         <v>23.920844585698628</v>
       </c>
     </row>
@@ -4312,27 +5711,27 @@
         <v>157984</v>
       </c>
       <c r="I40" s="2">
-        <f>1000000000/E40</f>
+        <f t="shared" si="6"/>
         <v>20108.990729755275</v>
       </c>
       <c r="J40" s="2">
-        <f>1000000000/G40</f>
+        <f t="shared" si="7"/>
         <v>3830.2142621858266</v>
       </c>
       <c r="K40" s="2">
-        <f>1000000000/H40</f>
+        <f t="shared" si="8"/>
         <v>6329.7549118898114</v>
       </c>
       <c r="L40" s="2">
-        <f>I40*4096/(1024*1024)</f>
+        <f t="shared" si="9"/>
         <v>78.550745038106541</v>
       </c>
       <c r="M40" s="2">
-        <f>J40*4096/(1024*1024)</f>
+        <f t="shared" si="10"/>
         <v>14.961774461663385</v>
       </c>
       <c r="N40" s="2">
-        <f>K40*4096/(1024*1024)</f>
+        <f t="shared" si="11"/>
         <v>24.725605124569576</v>
       </c>
     </row>
@@ -4362,27 +5761,27 @@
         <v>150486</v>
       </c>
       <c r="I41" s="2">
-        <f>1000000000/E41</f>
+        <f t="shared" si="6"/>
         <v>19535.065442469233</v>
       </c>
       <c r="J41" s="2">
-        <f>1000000000/G41</f>
+        <f t="shared" si="7"/>
         <v>3601.1509278365365</v>
       </c>
       <c r="K41" s="2">
-        <f>1000000000/H41</f>
+        <f t="shared" si="8"/>
         <v>6645.1364246507983</v>
       </c>
       <c r="L41" s="2">
-        <f>I41*4096/(1024*1024)</f>
+        <f t="shared" si="9"/>
         <v>76.308849384645441</v>
       </c>
       <c r="M41" s="2">
-        <f>J41*4096/(1024*1024)</f>
+        <f t="shared" si="10"/>
         <v>14.066995811861471</v>
       </c>
       <c r="N41" s="2">
-        <f>K41*4096/(1024*1024)</f>
+        <f t="shared" si="11"/>
         <v>25.957564158792181</v>
       </c>
     </row>
@@ -4412,27 +5811,27 @@
         <v>129980</v>
       </c>
       <c r="I42" s="2">
-        <f>1000000000/E42</f>
+        <f t="shared" si="6"/>
         <v>18832.746379404507</v>
       </c>
       <c r="J42" s="2">
-        <f>1000000000/G42</f>
+        <f t="shared" si="7"/>
         <v>3533.4565331844569</v>
       </c>
       <c r="K42" s="2">
-        <f>1000000000/H42</f>
+        <f t="shared" si="8"/>
         <v>7693.4913063548238</v>
       </c>
       <c r="L42" s="2">
-        <f>I42*4096/(1024*1024)</f>
+        <f t="shared" si="9"/>
         <v>73.565415544548856</v>
       </c>
       <c r="M42" s="2">
-        <f>J42*4096/(1024*1024)</f>
+        <f t="shared" si="10"/>
         <v>13.802564582751785</v>
       </c>
       <c r="N42" s="2">
-        <f>K42*4096/(1024*1024)</f>
+        <f t="shared" si="11"/>
         <v>30.05270041544853</v>
       </c>
     </row>
@@ -4462,27 +5861,27 @@
         <v>140024</v>
       </c>
       <c r="I43" s="2">
-        <f>1000000000/E43</f>
+        <f t="shared" si="6"/>
         <v>16376.260972094851</v>
       </c>
       <c r="J43" s="2">
-        <f>1000000000/G43</f>
+        <f t="shared" si="7"/>
         <v>4055.1664848600358</v>
       </c>
       <c r="K43" s="2">
-        <f>1000000000/H43</f>
+        <f t="shared" si="8"/>
         <v>7141.6328629377822</v>
       </c>
       <c r="L43" s="2">
-        <f>I43*4096/(1024*1024)</f>
+        <f t="shared" si="9"/>
         <v>63.969769422245513</v>
       </c>
       <c r="M43" s="2">
-        <f>J43*4096/(1024*1024)</f>
+        <f t="shared" si="10"/>
         <v>15.840494081484515</v>
       </c>
       <c r="N43" s="2">
-        <f>K43*4096/(1024*1024)</f>
+        <f t="shared" si="11"/>
         <v>27.897003370850712</v>
       </c>
     </row>
@@ -4512,27 +5911,27 @@
         <v>107830</v>
       </c>
       <c r="I44" s="2">
-        <f>1000000000/E44</f>
+        <f t="shared" si="6"/>
         <v>12861.074671399541</v>
       </c>
       <c r="J44" s="2">
-        <f>1000000000/G44</f>
+        <f t="shared" si="7"/>
         <v>4955.3522759933003</v>
       </c>
       <c r="K44" s="2">
-        <f>1000000000/H44</f>
+        <f t="shared" si="8"/>
         <v>9273.8569971251036</v>
       </c>
       <c r="L44" s="2">
-        <f>I44*4096/(1024*1024)</f>
+        <f t="shared" si="9"/>
         <v>50.238572935154458</v>
       </c>
       <c r="M44" s="2">
-        <f>J44*4096/(1024*1024)</f>
+        <f t="shared" si="10"/>
         <v>19.356844828098829</v>
       </c>
       <c r="N44" s="2">
-        <f>K44*4096/(1024*1024)</f>
+        <f t="shared" si="11"/>
         <v>36.226003895019936</v>
       </c>
     </row>
@@ -4562,27 +5961,27 @@
         <v>48460</v>
       </c>
       <c r="I45" s="2">
-        <f>1000000000/E45</f>
+        <f t="shared" si="6"/>
         <v>41106.589386278618</v>
       </c>
       <c r="J45" s="2">
-        <f>1000000000/G45</f>
+        <f t="shared" si="7"/>
         <v>23703.984639817954</v>
       </c>
       <c r="K45" s="2">
-        <f>1000000000/H45</f>
+        <f t="shared" si="8"/>
         <v>20635.575732562938</v>
       </c>
       <c r="L45" s="2">
-        <f>I45*4096/(1024*1024)</f>
+        <f t="shared" si="9"/>
         <v>160.57261479015085</v>
       </c>
       <c r="M45" s="2">
-        <f>J45*4096/(1024*1024)</f>
+        <f t="shared" si="10"/>
         <v>92.593689999288884</v>
       </c>
       <c r="N45" s="2">
-        <f>K45*4096/(1024*1024)</f>
+        <f t="shared" si="11"/>
         <v>80.607717705323978</v>
       </c>
     </row>
@@ -4612,27 +6011,27 @@
         <v>58742</v>
       </c>
       <c r="I46" s="2">
-        <f>1000000000/E46</f>
+        <f t="shared" si="6"/>
         <v>76057.195010648007</v>
       </c>
       <c r="J46" s="2">
-        <f>1000000000/G46</f>
+        <f t="shared" si="7"/>
         <v>36197.784695576629</v>
       </c>
       <c r="K46" s="2">
-        <f>1000000000/H46</f>
+        <f t="shared" si="8"/>
         <v>17023.594702257327</v>
       </c>
       <c r="L46" s="2">
-        <f>I46*4096/(1024*1024)</f>
+        <f t="shared" si="9"/>
         <v>297.09841801034378</v>
       </c>
       <c r="M46" s="2">
-        <f>J46*4096/(1024*1024)</f>
+        <f t="shared" si="10"/>
         <v>141.39759646709621</v>
       </c>
       <c r="N46" s="2">
-        <f>K46*4096/(1024*1024)</f>
+        <f t="shared" si="11"/>
         <v>66.498416805692685</v>
       </c>
     </row>
@@ -4662,27 +6061,27 @@
         <v>38344</v>
       </c>
       <c r="I47" s="2">
-        <f>1000000000/E47</f>
+        <f t="shared" si="6"/>
         <v>135685.21031207597</v>
       </c>
       <c r="J47" s="2">
-        <f>1000000000/G47</f>
+        <f t="shared" si="7"/>
         <v>58830.450641251911</v>
       </c>
       <c r="K47" s="2">
-        <f>1000000000/H47</f>
+        <f t="shared" si="8"/>
         <v>26079.699561861049</v>
       </c>
       <c r="L47" s="2">
-        <f>I47*4096/(1024*1024)</f>
+        <f t="shared" si="9"/>
         <v>530.02035278154676</v>
       </c>
       <c r="M47" s="2">
-        <f>J47*4096/(1024*1024)</f>
+        <f t="shared" si="10"/>
         <v>229.80644781739028</v>
       </c>
       <c r="N47" s="2">
-        <f>K47*4096/(1024*1024)</f>
+        <f t="shared" si="11"/>
         <v>101.87382641351972</v>
       </c>
     </row>
@@ -4712,27 +6111,27 @@
         <v>20986</v>
       </c>
       <c r="I48" s="2">
-        <f>1000000000/E48</f>
+        <f t="shared" si="6"/>
         <v>188323.91713747647</v>
       </c>
       <c r="J48" s="2">
-        <f>1000000000/G48</f>
+        <f t="shared" si="7"/>
         <v>82685.629237638495</v>
       </c>
       <c r="K48" s="2">
-        <f>1000000000/H48</f>
+        <f t="shared" si="8"/>
         <v>47650.814828933573</v>
       </c>
       <c r="L48" s="2">
-        <f>I48*4096/(1024*1024)</f>
+        <f t="shared" si="9"/>
         <v>735.64030131826746</v>
       </c>
       <c r="M48" s="2">
-        <f>J48*4096/(1024*1024)</f>
+        <f t="shared" si="10"/>
         <v>322.99073920952537</v>
       </c>
       <c r="N48" s="2">
-        <f>K48*4096/(1024*1024)</f>
+        <f t="shared" si="11"/>
         <v>186.13599542552177</v>
       </c>
     </row>
@@ -4762,27 +6161,27 @@
         <v>13241</v>
       </c>
       <c r="I49" s="2">
-        <f>1000000000/E49</f>
+        <f t="shared" si="6"/>
         <v>165043.73659019641</v>
       </c>
       <c r="J49" s="2">
-        <f>1000000000/G49</f>
+        <f t="shared" si="7"/>
         <v>95328.884652049572</v>
       </c>
       <c r="K49" s="2">
-        <f>1000000000/H49</f>
+        <f t="shared" si="8"/>
         <v>75522.996752511142</v>
       </c>
       <c r="L49" s="2">
-        <f>I49*4096/(1024*1024)</f>
+        <f t="shared" si="9"/>
         <v>644.70209605545472</v>
       </c>
       <c r="M49" s="2">
-        <f>J49*4096/(1024*1024)</f>
+        <f t="shared" si="10"/>
         <v>372.37845567206864</v>
       </c>
       <c r="N49" s="2">
-        <f>K49*4096/(1024*1024)</f>
+        <f t="shared" si="11"/>
         <v>295.01170606449665</v>
       </c>
     </row>
@@ -4812,27 +6211,27 @@
         <v>20866</v>
       </c>
       <c r="I50" s="2">
-        <f>1000000000/E50</f>
+        <f t="shared" si="6"/>
         <v>156274.4178777934</v>
       </c>
       <c r="J50" s="2">
-        <f>1000000000/G50</f>
+        <f t="shared" si="7"/>
         <v>89734.386216798273</v>
       </c>
       <c r="K50" s="2">
-        <f>1000000000/H50</f>
+        <f t="shared" si="8"/>
         <v>47924.853829195818</v>
       </c>
       <c r="L50" s="2">
-        <f>I50*4096/(1024*1024)</f>
+        <f t="shared" si="9"/>
         <v>610.44694483513047</v>
       </c>
       <c r="M50" s="2">
-        <f>J50*4096/(1024*1024)</f>
+        <f t="shared" si="10"/>
         <v>350.52494615936826</v>
       </c>
       <c r="N50" s="2">
-        <f>K50*4096/(1024*1024)</f>
+        <f t="shared" si="11"/>
         <v>187.20646027029616</v>
       </c>
     </row>
@@ -4862,27 +6261,27 @@
         <v>8975</v>
       </c>
       <c r="I51" s="2">
-        <f>1000000000/E51</f>
+        <f t="shared" si="6"/>
         <v>146241.59110851126</v>
       </c>
       <c r="J51" s="2">
-        <f>1000000000/G51</f>
+        <f t="shared" si="7"/>
         <v>102912.42152927858</v>
       </c>
       <c r="K51" s="2">
-        <f>1000000000/H51</f>
+        <f t="shared" si="8"/>
         <v>111420.61281337048</v>
       </c>
       <c r="L51" s="2">
-        <f>I51*4096/(1024*1024)</f>
+        <f t="shared" si="9"/>
         <v>571.25621526762211</v>
       </c>
       <c r="M51" s="2">
-        <f>J51*4096/(1024*1024)</f>
+        <f t="shared" si="10"/>
         <v>402.00164659874446</v>
       </c>
       <c r="N51" s="2">
-        <f>K51*4096/(1024*1024)</f>
+        <f t="shared" si="11"/>
         <v>435.23676880222843</v>
       </c>
     </row>
@@ -4912,27 +6311,27 @@
         <v>7020</v>
       </c>
       <c r="I52" s="2">
-        <f>1000000000/E52</f>
+        <f t="shared" si="6"/>
         <v>137249.51962668131</v>
       </c>
       <c r="J52" s="2">
-        <f>1000000000/G52</f>
+        <f t="shared" si="7"/>
         <v>121728.54534388315</v>
       </c>
       <c r="K52" s="2">
-        <f>1000000000/H52</f>
+        <f t="shared" si="8"/>
         <v>142450.14245014245</v>
       </c>
       <c r="L52" s="2">
-        <f>I52*4096/(1024*1024)</f>
+        <f t="shared" si="9"/>
         <v>536.13093604172388</v>
       </c>
       <c r="M52" s="2">
-        <f>J52*4096/(1024*1024)</f>
+        <f t="shared" si="10"/>
         <v>475.50213024954354</v>
       </c>
       <c r="N52" s="2">
-        <f>K52*4096/(1024*1024)</f>
+        <f t="shared" si="11"/>
         <v>556.44586894586894</v>
       </c>
     </row>
@@ -4962,28 +6361,48 @@
         <v>6836</v>
       </c>
       <c r="I53" s="2">
-        <f>1000000000/E53</f>
+        <f t="shared" si="6"/>
         <v>133440.08540165465</v>
       </c>
       <c r="J53" s="2">
-        <f>1000000000/G53</f>
+        <f t="shared" si="7"/>
         <v>138908.18169190164</v>
       </c>
       <c r="K53" s="2">
-        <f>1000000000/H53</f>
+        <f t="shared" si="8"/>
         <v>146284.3768285547</v>
       </c>
       <c r="L53" s="2">
-        <f>I53*4096/(1024*1024)</f>
+        <f t="shared" si="9"/>
         <v>521.25033360021348</v>
       </c>
       <c r="M53" s="2">
-        <f>J53*4096/(1024*1024)</f>
+        <f t="shared" si="10"/>
         <v>542.61008473399079</v>
       </c>
       <c r="N53" s="2">
-        <f>K53*4096/(1024*1024)</f>
+        <f t="shared" si="11"/>
         <v>571.42334698654179</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated graphs for all umap tests
</commit_message>
<xml_diff>
--- a/tests/pfbenchmark/test_results/data.xlsx
+++ b/tests/pfbenchmark/test_results/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcfadden8/umap/src/umap/tests/pfbenchmark/test_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235CA318-F790-E34F-99BD-44E9E393F48F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5E29B0-45DC-0849-BE19-35C4E8DA87F8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-51200" yWindow="-820" windowWidth="51200" windowHeight="31540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="26">
   <si>
     <t>test</t>
   </si>
@@ -86,6 +86,18 @@
   </si>
   <si>
     <t>1 UFFD Thread - Dirty Evictions</t>
+  </si>
+  <si>
+    <t>80 UFFD Threads -I/O</t>
+  </si>
+  <si>
+    <t>80 UFFD Threads +I/O</t>
+  </si>
+  <si>
+    <t>1 UFFD Thread -I/O</t>
+  </si>
+  <si>
+    <t>1 UFFD Thread +I/O</t>
   </si>
 </sst>
 </file>
@@ -1456,6 +1468,834 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t>UMAP Store (WP</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Fault)</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> Bandwidth</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>(4k</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Page Writes)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$A$61</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>80 UFFD Threads -I/O</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$C$27:$C$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$J$27:$J$35</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>24551.324543959148</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37335.722819593786</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53619.302949061661</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>77736.318407960192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>89405.453732677692</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>96983.803704781298</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>109158.38882218099</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>151883.35358444715</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>129971.40629061607</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FE4D-894B-8B12-F2A4039BC474}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$A$62</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>80 UFFD Threads +I/O</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$C$27:$C$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$J$45:$J$53</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>23703.984639817954</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36197.784695576629</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58830.450641251911</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>82685.629237638495</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>95328.884652049572</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>89734.386216798273</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>102912.42152927858</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>121728.54534388315</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>138908.18169190164</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FE4D-894B-8B12-F2A4039BC474}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$A$63</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1 UFFD Thread -I/O</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$C$27:$C$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$J$18:$J$26</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>46110.57315442431</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>73605.181804799053</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53070.105609510159</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>56401.579244218839</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>53516.00128438403</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>52648.204696219858</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45687.134502923975</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>38095.238095238092</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>29143.473319150176</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FE4D-894B-8B12-F2A4039BC474}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$A$64</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1 UFFD Thread +I/O</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$C$27:$C$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$J$36:$J$44</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>15420.200462606013</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5974.5365253290474</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4940.8091068993463</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3931.9149605432335</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3830.2142621858266</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3601.1509278365365</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3533.4565331844569</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4055.1664848600358</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4955.3522759933003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-FE4D-894B-8B12-F2A4039BC474}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1342641007"/>
+        <c:axId val="1441500303"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1342641007"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>OMP Threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1441500303"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1441500303"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>IOPS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1342641007"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>UMAP Eviction Bandwidth</a:t>
             </a:r>
             <a:r>
@@ -1610,7 +2450,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FE4D-894B-8B12-F2A4039BC474}"/>
+              <c16:uniqueId val="{00000000-8DB1-6F4A-9AB8-3682DC78A09B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1715,7 +2555,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-FE4D-894B-8B12-F2A4039BC474}"/>
+              <c16:uniqueId val="{00000001-8DB1-6F4A-9AB8-3682DC78A09B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1820,7 +2660,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-FE4D-894B-8B12-F2A4039BC474}"/>
+              <c16:uniqueId val="{00000002-8DB1-6F4A-9AB8-3682DC78A09B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1925,7 +2765,835 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-FE4D-894B-8B12-F2A4039BC474}"/>
+              <c16:uniqueId val="{00000003-8DB1-6F4A-9AB8-3682DC78A09B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1342641007"/>
+        <c:axId val="1441500303"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1342641007"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>OMP Threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1441500303"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1441500303"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>IOPS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1342641007"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>UMAP Store (Write</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Fault)</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> Bandwidth</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>(4k</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Page Writes)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$A$61</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>80 UFFD Threads -I/O</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$C$27:$C$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$E$27:$E$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>21591</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11679</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6713</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5757</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6481</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6633</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7105</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7040</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7478</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-488E-9349-8B2D-C30FDC49B01A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$A$62</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>80 UFFD Threads +I/O</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$C$27:$C$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$E$45:$E$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>24327</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13148</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7370</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5310</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6059</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6399</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6838</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7286</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7494</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-488E-9349-8B2D-C30FDC49B01A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$A$63</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1 UFFD Thread -I/O</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$C$27:$C$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$E$18:$E$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>21217</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14944</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16512</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16764</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17647</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18032</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20790</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24195</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33303</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-488E-9349-8B2D-C30FDC49B01A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$A$64</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1 UFFD Thread +I/O</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$C$27:$C$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$E$36:$E$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>54104</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53795</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>49787</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48619</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49729</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>51190</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>53099</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>61064</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>77754</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-488E-9349-8B2D-C30FDC49B01A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2321,6 +3989,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2838,6 +4586,1038 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3424,6 +6204,82 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>548819</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>43845</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5360F3AB-4A0F-A84A-9604-944E045360C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>105833</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>210152</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>149679</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11BA028E-149A-8E46-9689-39C7CE5D9C43}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3729,10 +6585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N59"/>
+  <dimension ref="A1:N64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+      <selection activeCell="O57" sqref="O57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6403,6 +9259,26 @@
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Import data into data.xlsx
</commit_message>
<xml_diff>
--- a/tests/pfbenchmark/test_results/data.xlsx
+++ b/tests/pfbenchmark/test_results/data.xlsx
@@ -5,22 +5,27 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcfadden8/umap/src/umap/tests/pfbenchmark/test_results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loki/umap/src/umap/tests/pfbenchmark/test_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5E29B0-45DC-0849-BE19-35C4E8DA87F8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B31234-6D08-494F-A3B7-95D7732EADB6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="-820" windowWidth="51200" windowHeight="31540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="7" r:id="rId1"/>
+    <sheet name="Read" sheetId="2" r:id="rId2"/>
+    <sheet name="RMW" sheetId="3" r:id="rId3"/>
+    <sheet name="Eviction" sheetId="4" r:id="rId4"/>
+    <sheet name="Write" sheetId="5" r:id="rId5"/>
+    <sheet name="data.old" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="29">
   <si>
     <t>test</t>
   </si>
@@ -98,6 +103,15 @@
   </si>
   <si>
     <t>1 UFFD Thread +I/O</t>
+  </si>
+  <si>
+    <t>read</t>
+  </si>
+  <si>
+    <t>write</t>
+  </si>
+  <si>
+    <t>nvme</t>
   </si>
 </sst>
 </file>
@@ -421,7 +435,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -536,6 +550,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -581,12 +675,24 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -753,7 +859,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$C$27:$C$35</c:f>
+              <c:f>data.old!$C$27:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -789,7 +895,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$K$27:$K$35</c:f>
+              <c:f>data.old!$K$27:$K$35</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="9"/>
@@ -826,7 +932,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000C-0009-C14A-8136-3E280810F71C}"/>
+              <c16:uniqueId val="{00000000-C3B9-FD4C-A421-50A64F6304ED}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -850,7 +956,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$C$27:$C$35</c:f>
+              <c:f>data.old!$C$27:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -886,7 +992,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$K$45:$K$53</c:f>
+              <c:f>data.old!$K$45:$K$53</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="9"/>
@@ -923,7 +1029,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000E-0009-C14A-8136-3E280810F71C}"/>
+              <c16:uniqueId val="{00000001-C3B9-FD4C-A421-50A64F6304ED}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -947,7 +1053,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$C$27:$C$35</c:f>
+              <c:f>data.old!$C$27:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -983,7 +1089,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$K$18:$K$26</c:f>
+              <c:f>data.old!$K$18:$K$26</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1020,7 +1126,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000D-0009-C14A-8136-3E280810F71C}"/>
+              <c16:uniqueId val="{00000002-C3B9-FD4C-A421-50A64F6304ED}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1044,7 +1150,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$C$27:$C$35</c:f>
+              <c:f>data.old!$C$27:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1080,7 +1186,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$K$36:$K$44</c:f>
+              <c:f>data.old!$K$36:$K$44</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1117,7 +1223,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000F-0009-C14A-8136-3E280810F71C}"/>
+              <c16:uniqueId val="{00000003-C3B9-FD4C-A421-50A64F6304ED}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1425,11 +1531,6 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -1534,7 +1635,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>data!$A$61</c:f>
+              <c:f>data.old!$A$79</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1557,7 +1658,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$C$27:$C$35</c:f>
+              <c:f>data.old!$C$27:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1593,7 +1694,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$J$27:$J$35</c:f>
+              <c:f>data.old!$J$27:$J$35</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1630,7 +1731,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FE4D-894B-8B12-F2A4039BC474}"/>
+              <c16:uniqueId val="{00000000-6528-BA4C-A84C-4D96691CCCCA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1639,7 +1740,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>data!$A$62</c:f>
+              <c:f>data.old!$A$80</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1662,7 +1763,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$C$27:$C$35</c:f>
+              <c:f>data.old!$C$27:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1698,7 +1799,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$J$45:$J$53</c:f>
+              <c:f>data.old!$J$45:$J$53</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1735,7 +1836,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-FE4D-894B-8B12-F2A4039BC474}"/>
+              <c16:uniqueId val="{00000001-6528-BA4C-A84C-4D96691CCCCA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1744,7 +1845,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>data!$A$63</c:f>
+              <c:f>data.old!$A$81</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1767,7 +1868,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$C$27:$C$35</c:f>
+              <c:f>data.old!$C$27:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1803,7 +1904,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$J$18:$J$26</c:f>
+              <c:f>data.old!$J$18:$J$26</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1840,7 +1941,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-FE4D-894B-8B12-F2A4039BC474}"/>
+              <c16:uniqueId val="{00000002-6528-BA4C-A84C-4D96691CCCCA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1849,7 +1950,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>data!$A$64</c:f>
+              <c:f>data.old!$A$82</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1872,7 +1973,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$C$27:$C$35</c:f>
+              <c:f>data.old!$C$27:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1908,7 +2009,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$J$36:$J$44</c:f>
+              <c:f>data.old!$J$36:$J$44</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1945,7 +2046,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-FE4D-894B-8B12-F2A4039BC474}"/>
+              <c16:uniqueId val="{00000003-6528-BA4C-A84C-4D96691CCCCA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2253,11 +2354,6 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -2354,7 +2450,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>data!$A$56</c:f>
+              <c:f>data.old!$A$74</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2377,7 +2473,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$C$27:$C$35</c:f>
+              <c:f>data.old!$C$27:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2413,7 +2509,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$F$27:$F$35</c:f>
+              <c:f>data.old!$F$27:$F$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2450,7 +2546,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8DB1-6F4A-9AB8-3682DC78A09B}"/>
+              <c16:uniqueId val="{00000000-C77C-C64D-8DC1-EE2E967FAE6A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2459,7 +2555,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>data!$A$57</c:f>
+              <c:f>data.old!$A$75</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2482,7 +2578,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$C$27:$C$35</c:f>
+              <c:f>data.old!$C$27:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2518,7 +2614,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$F$45:$F$53</c:f>
+              <c:f>data.old!$F$45:$F$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2555,7 +2651,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8DB1-6F4A-9AB8-3682DC78A09B}"/>
+              <c16:uniqueId val="{00000001-C77C-C64D-8DC1-EE2E967FAE6A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2564,7 +2660,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>data!$A$58</c:f>
+              <c:f>data.old!$A$76</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2587,7 +2683,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$C$27:$C$35</c:f>
+              <c:f>data.old!$C$27:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2623,7 +2719,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$F$18:$F$26</c:f>
+              <c:f>data.old!$F$18:$F$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2660,7 +2756,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-8DB1-6F4A-9AB8-3682DC78A09B}"/>
+              <c16:uniqueId val="{00000002-C77C-C64D-8DC1-EE2E967FAE6A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2669,7 +2765,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>data!$A$59</c:f>
+              <c:f>data.old!$A$77</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2692,7 +2788,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$C$27:$C$35</c:f>
+              <c:f>data.old!$C$27:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2728,7 +2824,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$F$36:$F$44</c:f>
+              <c:f>data.old!$F$36:$F$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2765,7 +2861,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-8DB1-6F4A-9AB8-3682DC78A09B}"/>
+              <c16:uniqueId val="{00000003-C77C-C64D-8DC1-EE2E967FAE6A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3073,11 +3169,6 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -3182,7 +3273,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>data!$A$61</c:f>
+              <c:f>data.old!$A$79</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3205,7 +3296,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$C$27:$C$35</c:f>
+              <c:f>data.old!$C$27:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -3241,7 +3332,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$E$27:$E$35</c:f>
+              <c:f>data.old!$E$27:$E$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -3278,7 +3369,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-488E-9349-8B2D-C30FDC49B01A}"/>
+              <c16:uniqueId val="{00000000-F53E-6F47-A0E5-0D3A39F3A629}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3287,7 +3378,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>data!$A$62</c:f>
+              <c:f>data.old!$A$80</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3310,7 +3401,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$C$27:$C$35</c:f>
+              <c:f>data.old!$C$27:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -3346,7 +3437,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$E$45:$E$53</c:f>
+              <c:f>data.old!$E$45:$E$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -3383,7 +3474,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-488E-9349-8B2D-C30FDC49B01A}"/>
+              <c16:uniqueId val="{00000001-F53E-6F47-A0E5-0D3A39F3A629}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3392,7 +3483,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>data!$A$63</c:f>
+              <c:f>data.old!$A$81</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3415,7 +3506,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$C$27:$C$35</c:f>
+              <c:f>data.old!$C$27:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -3451,7 +3542,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$E$18:$E$26</c:f>
+              <c:f>data.old!$E$18:$E$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -3488,7 +3579,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-488E-9349-8B2D-C30FDC49B01A}"/>
+              <c16:uniqueId val="{00000002-F53E-6F47-A0E5-0D3A39F3A629}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3497,7 +3588,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>data!$A$64</c:f>
+              <c:f>data.old!$A$82</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3520,7 +3611,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$C$27:$C$35</c:f>
+              <c:f>data.old!$C$27:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -3556,7 +3647,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$E$36:$E$44</c:f>
+              <c:f>data.old!$E$36:$E$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -3593,7 +3684,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-488E-9349-8B2D-C30FDC49B01A}"/>
+              <c16:uniqueId val="{00000003-F53E-6F47-A0E5-0D3A39F3A629}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3901,11 +3992,6 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -6133,31 +6219,67 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{962B71A9-70A2-094F-942C-93F9CF7B6D6F}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="237" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{D745799B-C46A-CD46-8B71-860347A44F60}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="237" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{C07207E0-1970-8D42-9FEE-DFA101531B6F}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="237" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{2BC7DB60-C0F0-A146-96AD-A703487C6965}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="237" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>512538</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>151191</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>542773</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>195036</xdr:rowOff>
-    </xdr:to>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8681013" cy="6291055"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80F90FDA-6746-9D4E-B5DA-F6311665CFCE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA5A3DB4-DFE0-FB40-8564-21E23A0362C1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -6170,31 +6292,26 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>30235</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>43846</xdr:rowOff>
-    </xdr:to>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8681013" cy="6291055"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F3F5F96-995C-A942-94A7-05EBA14725CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0E0BA9A-66C1-A34A-A894-D32C8829126D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
+          <a:graphicFrameLocks noGrp="1"/>
         </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6203,36 +6320,31 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>548819</xdr:colOff>
-      <xdr:row>101</xdr:row>
-      <xdr:rowOff>43845</xdr:rowOff>
-    </xdr:to>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8681013" cy="6291055"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5360F3AB-4A0F-A84A-9604-944E045360C9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98483F48-535D-764A-A2FF-D08FEBF28B9E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
+          <a:graphicFrameLocks noGrp="1"/>
         </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6241,36 +6353,31 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>698500</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>105833</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>210152</xdr:colOff>
-      <xdr:row>94</xdr:row>
-      <xdr:rowOff>149679</xdr:rowOff>
-    </xdr:to>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8681013" cy="6291055"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11BA028E-149A-8E46-9689-39C7CE5D9C43}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BF87017-E859-CC47-93D8-F9681066E4C3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
+          <a:graphicFrameLocks noGrp="1"/>
         </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6279,12 +6386,12 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6584,11 +6691,1830 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{691F6356-0BAB-364F-B876-A302712E1823}">
+  <dimension ref="A1:AO20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.6640625" customWidth="1"/>
+    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.6640625" customWidth="1"/>
+    <col min="15" max="15" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.33203125" customWidth="1"/>
+    <col min="22" max="22" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.83203125" customWidth="1"/>
+    <col min="28" max="28" width="3.1640625" customWidth="1"/>
+    <col min="29" max="29" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="2.83203125" customWidth="1"/>
+    <col min="36" max="36" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="6.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:41" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="2"/>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="12">
+        <v>1</v>
+      </c>
+      <c r="E2" s="12">
+        <v>0</v>
+      </c>
+      <c r="F2" s="9">
+        <v>21971</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="12">
+        <v>1</v>
+      </c>
+      <c r="L2" s="12">
+        <v>1</v>
+      </c>
+      <c r="M2" s="9">
+        <v>79260</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" s="12">
+        <v>1</v>
+      </c>
+      <c r="S2" s="12">
+        <v>1</v>
+      </c>
+      <c r="T2" s="9">
+        <v>28770</v>
+      </c>
+      <c r="U2" s="13"/>
+      <c r="V2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y2" s="12">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="9">
+        <v>16938</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF2" s="12">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="12">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="9">
+        <v>57233</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM2" s="12">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="12">
+        <v>1</v>
+      </c>
+      <c r="AO2" s="9">
+        <v>20047</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="13">
+        <v>2</v>
+      </c>
+      <c r="E3" s="13">
+        <v>0</v>
+      </c>
+      <c r="F3" s="10">
+        <v>13116</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="13">
+        <v>2</v>
+      </c>
+      <c r="L3" s="13">
+        <v>1</v>
+      </c>
+      <c r="M3" s="10">
+        <v>61331</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="R3" s="13">
+        <v>2</v>
+      </c>
+      <c r="S3" s="13">
+        <v>1</v>
+      </c>
+      <c r="T3" s="10">
+        <v>15512</v>
+      </c>
+      <c r="U3" s="13"/>
+      <c r="V3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="W3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y3" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="10">
+        <v>50709</v>
+      </c>
+      <c r="AC3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF3" s="13">
+        <v>2</v>
+      </c>
+      <c r="AG3" s="13">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="10">
+        <v>167444</v>
+      </c>
+      <c r="AJ3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM3" s="13">
+        <v>2</v>
+      </c>
+      <c r="AN3" s="13">
+        <v>1</v>
+      </c>
+      <c r="AO3" s="10">
+        <v>15943</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="13">
+        <v>4</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10">
+        <v>15470</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="13">
+        <v>4</v>
+      </c>
+      <c r="L4" s="13">
+        <v>1</v>
+      </c>
+      <c r="M4" s="10">
+        <v>59697</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="R4" s="13">
+        <v>4</v>
+      </c>
+      <c r="S4" s="13">
+        <v>1</v>
+      </c>
+      <c r="T4" s="10">
+        <v>16593</v>
+      </c>
+      <c r="U4" s="13"/>
+      <c r="V4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="W4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y4" s="13">
+        <v>4</v>
+      </c>
+      <c r="Z4" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="10">
+        <v>29905</v>
+      </c>
+      <c r="AC4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF4" s="13">
+        <v>4</v>
+      </c>
+      <c r="AG4" s="13">
+        <v>1</v>
+      </c>
+      <c r="AH4" s="10">
+        <v>168454</v>
+      </c>
+      <c r="AJ4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM4" s="13">
+        <v>4</v>
+      </c>
+      <c r="AN4" s="13">
+        <v>1</v>
+      </c>
+      <c r="AO4" s="10">
+        <v>13392</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="13">
+        <v>8</v>
+      </c>
+      <c r="E5" s="13">
+        <v>0</v>
+      </c>
+      <c r="F5" s="10">
+        <v>40439</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="13">
+        <v>8</v>
+      </c>
+      <c r="L5" s="13">
+        <v>1</v>
+      </c>
+      <c r="M5" s="10">
+        <v>58671</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="R5" s="13">
+        <v>8</v>
+      </c>
+      <c r="S5" s="13">
+        <v>1</v>
+      </c>
+      <c r="T5" s="10">
+        <v>16598</v>
+      </c>
+      <c r="U5" s="13"/>
+      <c r="V5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="W5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y5" s="13">
+        <v>8</v>
+      </c>
+      <c r="Z5" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="10">
+        <v>17063</v>
+      </c>
+      <c r="AC5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF5" s="13">
+        <v>8</v>
+      </c>
+      <c r="AG5" s="13">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="10">
+        <v>170609</v>
+      </c>
+      <c r="AJ5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM5" s="13">
+        <v>8</v>
+      </c>
+      <c r="AN5" s="13">
+        <v>1</v>
+      </c>
+      <c r="AO5" s="10">
+        <v>12724</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="13">
+        <v>16</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0</v>
+      </c>
+      <c r="F6" s="10">
+        <v>43520</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="13">
+        <v>16</v>
+      </c>
+      <c r="L6" s="13">
+        <v>1</v>
+      </c>
+      <c r="M6" s="10">
+        <v>58191</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="R6" s="13">
+        <v>16</v>
+      </c>
+      <c r="S6" s="13">
+        <v>1</v>
+      </c>
+      <c r="T6" s="10">
+        <v>17169</v>
+      </c>
+      <c r="U6" s="13"/>
+      <c r="V6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="W6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y6" s="13">
+        <v>16</v>
+      </c>
+      <c r="Z6" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="10">
+        <v>25577</v>
+      </c>
+      <c r="AC6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF6" s="13">
+        <v>16</v>
+      </c>
+      <c r="AG6" s="13">
+        <v>1</v>
+      </c>
+      <c r="AH6" s="10">
+        <v>142237</v>
+      </c>
+      <c r="AJ6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM6" s="13">
+        <v>16</v>
+      </c>
+      <c r="AN6" s="13">
+        <v>1</v>
+      </c>
+      <c r="AO6" s="10">
+        <v>13641</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="13">
+        <v>32</v>
+      </c>
+      <c r="E7" s="13">
+        <v>0</v>
+      </c>
+      <c r="F7" s="10">
+        <v>56306</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="13">
+        <v>32</v>
+      </c>
+      <c r="L7" s="13">
+        <v>1</v>
+      </c>
+      <c r="M7" s="10">
+        <v>58040</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="R7" s="13">
+        <v>32</v>
+      </c>
+      <c r="S7" s="13">
+        <v>1</v>
+      </c>
+      <c r="T7" s="10">
+        <v>18209</v>
+      </c>
+      <c r="U7" s="13"/>
+      <c r="V7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="W7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y7" s="13">
+        <v>32</v>
+      </c>
+      <c r="Z7" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="10">
+        <v>28230</v>
+      </c>
+      <c r="AC7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF7" s="13">
+        <v>32</v>
+      </c>
+      <c r="AG7" s="13">
+        <v>1</v>
+      </c>
+      <c r="AH7" s="10">
+        <v>130545</v>
+      </c>
+      <c r="AJ7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM7" s="13">
+        <v>32</v>
+      </c>
+      <c r="AN7" s="13">
+        <v>1</v>
+      </c>
+      <c r="AO7" s="10">
+        <v>14163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="13">
+        <v>64</v>
+      </c>
+      <c r="E8" s="13">
+        <v>0</v>
+      </c>
+      <c r="F8" s="10">
+        <v>52939</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="13">
+        <v>64</v>
+      </c>
+      <c r="L8" s="13">
+        <v>1</v>
+      </c>
+      <c r="M8" s="10">
+        <v>62166</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="R8" s="13">
+        <v>64</v>
+      </c>
+      <c r="S8" s="13">
+        <v>1</v>
+      </c>
+      <c r="T8" s="10">
+        <v>20247</v>
+      </c>
+      <c r="U8" s="13"/>
+      <c r="V8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="W8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y8" s="13">
+        <v>64</v>
+      </c>
+      <c r="Z8" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="10">
+        <v>29746</v>
+      </c>
+      <c r="AC8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF8" s="13">
+        <v>64</v>
+      </c>
+      <c r="AG8" s="13">
+        <v>1</v>
+      </c>
+      <c r="AH8" s="10">
+        <v>151478</v>
+      </c>
+      <c r="AJ8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM8" s="13">
+        <v>64</v>
+      </c>
+      <c r="AN8" s="13">
+        <v>1</v>
+      </c>
+      <c r="AO8" s="10">
+        <v>15924</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="13">
+        <v>128</v>
+      </c>
+      <c r="E9" s="13">
+        <v>0</v>
+      </c>
+      <c r="F9" s="10">
+        <v>57270</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" s="13">
+        <v>128</v>
+      </c>
+      <c r="L9" s="13">
+        <v>1</v>
+      </c>
+      <c r="M9" s="10">
+        <v>69126</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="R9" s="13">
+        <v>128</v>
+      </c>
+      <c r="S9" s="13">
+        <v>1</v>
+      </c>
+      <c r="T9" s="10">
+        <v>25798</v>
+      </c>
+      <c r="U9" s="13"/>
+      <c r="V9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="W9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y9" s="13">
+        <v>128</v>
+      </c>
+      <c r="Z9" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="10">
+        <v>21215</v>
+      </c>
+      <c r="AC9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF9" s="13">
+        <v>128</v>
+      </c>
+      <c r="AG9" s="13">
+        <v>1</v>
+      </c>
+      <c r="AH9" s="10">
+        <v>156875</v>
+      </c>
+      <c r="AJ9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM9" s="13">
+        <v>128</v>
+      </c>
+      <c r="AN9" s="13">
+        <v>1</v>
+      </c>
+      <c r="AO9" s="10">
+        <v>18340</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="14">
+        <v>256</v>
+      </c>
+      <c r="E10" s="14">
+        <v>0</v>
+      </c>
+      <c r="F10" s="11">
+        <v>60000</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="14">
+        <v>256</v>
+      </c>
+      <c r="L10" s="14">
+        <v>1</v>
+      </c>
+      <c r="M10" s="11">
+        <v>82724</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="P10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q10" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="R10" s="14">
+        <v>256</v>
+      </c>
+      <c r="S10" s="14">
+        <v>1</v>
+      </c>
+      <c r="T10" s="11">
+        <v>34311</v>
+      </c>
+      <c r="U10" s="13"/>
+      <c r="V10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="W10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="X10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y10" s="14">
+        <v>256</v>
+      </c>
+      <c r="Z10" s="14">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="11">
+        <v>13947</v>
+      </c>
+      <c r="AC10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF10" s="14">
+        <v>256</v>
+      </c>
+      <c r="AG10" s="14">
+        <v>1</v>
+      </c>
+      <c r="AH10" s="11">
+        <v>131400</v>
+      </c>
+      <c r="AJ10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM10" s="14">
+        <v>256</v>
+      </c>
+      <c r="AN10" s="14">
+        <v>1</v>
+      </c>
+      <c r="AO10" s="11">
+        <v>22765</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
+      <c r="AF11" s="2"/>
+      <c r="AG11" s="2"/>
+      <c r="AH11" s="2"/>
+      <c r="AM11" s="2"/>
+      <c r="AN11" s="2"/>
+      <c r="AO11" s="2"/>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="H12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" s="12">
+        <v>1</v>
+      </c>
+      <c r="L12" s="12">
+        <v>80</v>
+      </c>
+      <c r="M12" s="9">
+        <v>81092</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="R12" s="12">
+        <v>1</v>
+      </c>
+      <c r="S12" s="12">
+        <v>80</v>
+      </c>
+      <c r="T12" s="9">
+        <v>25391</v>
+      </c>
+      <c r="U12" s="13"/>
+      <c r="V12" s="13"/>
+      <c r="W12" s="13"/>
+      <c r="X12" s="13"/>
+      <c r="Y12" s="13"/>
+      <c r="Z12" s="13"/>
+      <c r="AA12" s="13"/>
+      <c r="AC12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF12" s="12">
+        <v>1</v>
+      </c>
+      <c r="AG12" s="12">
+        <v>80</v>
+      </c>
+      <c r="AH12" s="9">
+        <v>52899</v>
+      </c>
+      <c r="AJ12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM12" s="12">
+        <v>1</v>
+      </c>
+      <c r="AN12" s="12">
+        <v>80</v>
+      </c>
+      <c r="AO12" s="9">
+        <v>23505</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="H13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K13" s="13">
+        <v>2</v>
+      </c>
+      <c r="L13" s="13">
+        <v>80</v>
+      </c>
+      <c r="M13" s="10">
+        <v>56785</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="R13" s="13">
+        <v>2</v>
+      </c>
+      <c r="S13" s="13">
+        <v>80</v>
+      </c>
+      <c r="T13" s="10">
+        <v>19000</v>
+      </c>
+      <c r="U13" s="13"/>
+      <c r="V13" s="13"/>
+      <c r="W13" s="13"/>
+      <c r="X13" s="13"/>
+      <c r="Y13" s="13"/>
+      <c r="Z13" s="13"/>
+      <c r="AA13" s="13"/>
+      <c r="AC13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF13" s="13">
+        <v>2</v>
+      </c>
+      <c r="AG13" s="13">
+        <v>80</v>
+      </c>
+      <c r="AH13" s="10">
+        <v>96013</v>
+      </c>
+      <c r="AJ13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM13" s="13">
+        <v>2</v>
+      </c>
+      <c r="AN13" s="13">
+        <v>80</v>
+      </c>
+      <c r="AO13" s="10">
+        <v>16135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="H14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K14" s="13">
+        <v>4</v>
+      </c>
+      <c r="L14" s="13">
+        <v>80</v>
+      </c>
+      <c r="M14" s="10">
+        <v>47030</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="R14" s="13">
+        <v>4</v>
+      </c>
+      <c r="S14" s="13">
+        <v>80</v>
+      </c>
+      <c r="T14" s="10">
+        <v>13616</v>
+      </c>
+      <c r="U14" s="13"/>
+      <c r="V14" s="13"/>
+      <c r="W14" s="13"/>
+      <c r="X14" s="13"/>
+      <c r="Y14" s="13"/>
+      <c r="Z14" s="13"/>
+      <c r="AA14" s="13"/>
+      <c r="AC14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF14" s="13">
+        <v>4</v>
+      </c>
+      <c r="AG14" s="13">
+        <v>80</v>
+      </c>
+      <c r="AH14" s="10">
+        <v>60022</v>
+      </c>
+      <c r="AJ14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM14" s="13">
+        <v>4</v>
+      </c>
+      <c r="AN14" s="13">
+        <v>80</v>
+      </c>
+      <c r="AO14" s="10">
+        <v>10953</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="H15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" s="13">
+        <v>8</v>
+      </c>
+      <c r="L15" s="13">
+        <v>80</v>
+      </c>
+      <c r="M15" s="10">
+        <v>32315</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="R15" s="13">
+        <v>8</v>
+      </c>
+      <c r="S15" s="13">
+        <v>80</v>
+      </c>
+      <c r="T15" s="10">
+        <v>9980</v>
+      </c>
+      <c r="U15" s="13"/>
+      <c r="V15" s="13"/>
+      <c r="W15" s="13"/>
+      <c r="X15" s="13"/>
+      <c r="Y15" s="13"/>
+      <c r="Z15" s="13"/>
+      <c r="AA15" s="13"/>
+      <c r="AC15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF15" s="13">
+        <v>8</v>
+      </c>
+      <c r="AG15" s="13">
+        <v>80</v>
+      </c>
+      <c r="AH15" s="10">
+        <v>38670</v>
+      </c>
+      <c r="AJ15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM15" s="13">
+        <v>8</v>
+      </c>
+      <c r="AN15" s="13">
+        <v>80</v>
+      </c>
+      <c r="AO15" s="10">
+        <v>7804</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="H16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16" s="13">
+        <v>16</v>
+      </c>
+      <c r="L16" s="13">
+        <v>80</v>
+      </c>
+      <c r="M16" s="10">
+        <v>81100</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="R16" s="13">
+        <v>16</v>
+      </c>
+      <c r="S16" s="13">
+        <v>80</v>
+      </c>
+      <c r="T16" s="10">
+        <v>8874</v>
+      </c>
+      <c r="U16" s="13"/>
+      <c r="V16" s="13"/>
+      <c r="W16" s="13"/>
+      <c r="X16" s="13"/>
+      <c r="Y16" s="13"/>
+      <c r="Z16" s="13"/>
+      <c r="AA16" s="13"/>
+      <c r="AC16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF16" s="13">
+        <v>16</v>
+      </c>
+      <c r="AG16" s="13">
+        <v>80</v>
+      </c>
+      <c r="AH16" s="10">
+        <v>30535</v>
+      </c>
+      <c r="AJ16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM16" s="13">
+        <v>16</v>
+      </c>
+      <c r="AN16" s="13">
+        <v>80</v>
+      </c>
+      <c r="AO16" s="10">
+        <v>6701</v>
+      </c>
+    </row>
+    <row r="17" spans="8:41" x14ac:dyDescent="0.2">
+      <c r="H17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K17" s="13">
+        <v>32</v>
+      </c>
+      <c r="L17" s="13">
+        <v>80</v>
+      </c>
+      <c r="M17" s="10">
+        <v>98773</v>
+      </c>
+      <c r="O17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="R17" s="13">
+        <v>32</v>
+      </c>
+      <c r="S17" s="13">
+        <v>80</v>
+      </c>
+      <c r="T17" s="10">
+        <v>8809</v>
+      </c>
+      <c r="U17" s="13"/>
+      <c r="V17" s="13"/>
+      <c r="W17" s="13"/>
+      <c r="X17" s="13"/>
+      <c r="Y17" s="13"/>
+      <c r="Z17" s="13"/>
+      <c r="AA17" s="13"/>
+      <c r="AC17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF17" s="13">
+        <v>32</v>
+      </c>
+      <c r="AG17" s="13">
+        <v>80</v>
+      </c>
+      <c r="AH17" s="10">
+        <v>26595</v>
+      </c>
+      <c r="AJ17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM17" s="13">
+        <v>32</v>
+      </c>
+      <c r="AN17" s="13">
+        <v>80</v>
+      </c>
+      <c r="AO17" s="10">
+        <v>7606</v>
+      </c>
+    </row>
+    <row r="18" spans="8:41" x14ac:dyDescent="0.2">
+      <c r="H18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K18" s="13">
+        <v>64</v>
+      </c>
+      <c r="L18" s="13">
+        <v>80</v>
+      </c>
+      <c r="M18" s="10">
+        <v>105481</v>
+      </c>
+      <c r="O18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="R18" s="13">
+        <v>64</v>
+      </c>
+      <c r="S18" s="13">
+        <v>80</v>
+      </c>
+      <c r="T18" s="10">
+        <v>8894</v>
+      </c>
+      <c r="U18" s="13"/>
+      <c r="V18" s="13"/>
+      <c r="W18" s="13"/>
+      <c r="X18" s="13"/>
+      <c r="Y18" s="13"/>
+      <c r="Z18" s="13"/>
+      <c r="AA18" s="13"/>
+      <c r="AC18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE18" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF18" s="13">
+        <v>64</v>
+      </c>
+      <c r="AG18" s="13">
+        <v>80</v>
+      </c>
+      <c r="AH18" s="10">
+        <v>10502</v>
+      </c>
+      <c r="AJ18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL18" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM18" s="13">
+        <v>64</v>
+      </c>
+      <c r="AN18" s="13">
+        <v>80</v>
+      </c>
+      <c r="AO18" s="10">
+        <v>7068</v>
+      </c>
+    </row>
+    <row r="19" spans="8:41" x14ac:dyDescent="0.2">
+      <c r="H19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K19" s="13">
+        <v>128</v>
+      </c>
+      <c r="L19" s="13">
+        <v>80</v>
+      </c>
+      <c r="M19" s="10">
+        <v>105434</v>
+      </c>
+      <c r="O19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="R19" s="13">
+        <v>128</v>
+      </c>
+      <c r="S19" s="13">
+        <v>80</v>
+      </c>
+      <c r="T19" s="10">
+        <v>7903</v>
+      </c>
+      <c r="U19" s="13"/>
+      <c r="V19" s="13"/>
+      <c r="W19" s="13"/>
+      <c r="X19" s="13"/>
+      <c r="Y19" s="13"/>
+      <c r="Z19" s="13"/>
+      <c r="AA19" s="13"/>
+      <c r="AC19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE19" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF19" s="13">
+        <v>128</v>
+      </c>
+      <c r="AG19" s="13">
+        <v>80</v>
+      </c>
+      <c r="AH19" s="10">
+        <v>7981</v>
+      </c>
+      <c r="AJ19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL19" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM19" s="13">
+        <v>128</v>
+      </c>
+      <c r="AN19" s="13">
+        <v>80</v>
+      </c>
+      <c r="AO19" s="10">
+        <v>6007</v>
+      </c>
+    </row>
+    <row r="20" spans="8:41" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H20" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K20" s="14">
+        <v>256</v>
+      </c>
+      <c r="L20" s="14">
+        <v>80</v>
+      </c>
+      <c r="M20" s="11">
+        <v>100657</v>
+      </c>
+      <c r="O20" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="P20" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q20" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="R20" s="14">
+        <v>256</v>
+      </c>
+      <c r="S20" s="14">
+        <v>80</v>
+      </c>
+      <c r="T20" s="11">
+        <v>7122</v>
+      </c>
+      <c r="U20" s="13"/>
+      <c r="V20" s="13"/>
+      <c r="W20" s="13"/>
+      <c r="X20" s="13"/>
+      <c r="Y20" s="13"/>
+      <c r="Z20" s="13"/>
+      <c r="AA20" s="13"/>
+      <c r="AC20" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD20" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE20" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF20" s="14">
+        <v>256</v>
+      </c>
+      <c r="AG20" s="14">
+        <v>80</v>
+      </c>
+      <c r="AH20" s="11">
+        <v>7591</v>
+      </c>
+      <c r="AJ20" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK20" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL20" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM20" s="14">
+        <v>256</v>
+      </c>
+      <c r="AN20" s="14">
+        <v>80</v>
+      </c>
+      <c r="AO20" s="11">
+        <v>5553</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N64"/>
+  <dimension ref="A1:N82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O57" sqref="O57"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9241,43 +11167,187 @@
         <v>571.42334698654179</v>
       </c>
     </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+      <c r="M54" s="2"/>
+      <c r="N54" s="2"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+      <c r="M55" s="2"/>
+      <c r="N55" s="2"/>
+    </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>18</v>
-      </c>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+      <c r="M56" s="2"/>
+      <c r="N56" s="2"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>19</v>
-      </c>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+      <c r="L57" s="2"/>
+      <c r="M57" s="2"/>
+      <c r="N57" s="2"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>20</v>
-      </c>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2"/>
+      <c r="L58" s="2"/>
+      <c r="M58" s="2"/>
+      <c r="N58" s="2"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>21</v>
-      </c>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="2"/>
+      <c r="L59" s="2"/>
+      <c r="M59" s="2"/>
+      <c r="N59" s="2"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
+      <c r="K60" s="2"/>
+      <c r="L60" s="2"/>
+      <c r="M60" s="2"/>
+      <c r="N60" s="2"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>22</v>
-      </c>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2"/>
+      <c r="K61" s="2"/>
+      <c r="L61" s="2"/>
+      <c r="M61" s="2"/>
+      <c r="N61" s="2"/>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>23</v>
-      </c>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
+      <c r="L62" s="2"/>
+      <c r="M62" s="2"/>
+      <c r="N62" s="2"/>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>24</v>
-      </c>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
+      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
+      <c r="M63" s="2"/>
+      <c r="N63" s="2"/>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+      <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
+      <c r="K64" s="2"/>
+      <c r="L64" s="2"/>
+      <c r="M64" s="2"/>
+      <c r="N64" s="2"/>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+      <c r="K65" s="2"/>
+      <c r="L65" s="2"/>
+      <c r="M65" s="2"/>
+      <c r="N65" s="2"/>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I66" s="2"/>
+      <c r="J66" s="2"/>
+      <c r="K66" s="2"/>
+      <c r="L66" s="2"/>
+      <c r="M66" s="2"/>
+      <c r="N66" s="2"/>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I67" s="2"/>
+      <c r="J67" s="2"/>
+      <c r="K67" s="2"/>
+      <c r="L67" s="2"/>
+      <c r="M67" s="2"/>
+      <c r="N67" s="2"/>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I68" s="2"/>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2"/>
+      <c r="L68" s="2"/>
+      <c r="M68" s="2"/>
+      <c r="N68" s="2"/>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I69" s="2"/>
+      <c r="J69" s="2"/>
+      <c r="K69" s="2"/>
+      <c r="L69" s="2"/>
+      <c r="M69" s="2"/>
+      <c r="N69" s="2"/>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I70" s="2"/>
+      <c r="J70" s="2"/>
+      <c r="K70" s="2"/>
+      <c r="L70" s="2"/>
+      <c r="M70" s="2"/>
+      <c r="N70" s="2"/>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I71" s="2"/>
+      <c r="J71" s="2"/>
+      <c r="K71" s="2"/>
+      <c r="L71" s="2"/>
+      <c r="M71" s="2"/>
+      <c r="N71" s="2"/>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>25</v>
       </c>
     </row>
@@ -9289,6 +11359,5 @@
     <sortCondition ref="C2:C53"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated graphs with better colors to differentiate curves
</commit_message>
<xml_diff>
--- a/tests/pfbenchmark/test_results/data.xlsx
+++ b/tests/pfbenchmark/test_results/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loki/umap/src/umap/tests/pfbenchmark/test_results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcfadden8/umap/src/umap/tests/pfbenchmark/test_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5209AC-F785-0342-84E4-5485C4E658A9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF42ECF-A21D-D24A-ABA6-1855CBA65D67}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-51220" yWindow="-520" windowWidth="50700" windowHeight="27840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="7" r:id="rId1"/>
@@ -784,15 +784,15 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="4"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>data!$A$1</c:f>
+              <c:f>data!$Q$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>NVME DirectIO</c:v>
+                  <c:v>UMAP -IO 80 UFFD Threads</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -800,7 +800,113 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$T$13:$T$21</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$W$13:$W$21</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>39384.03371273286</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52631.57894736842</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>73443.008225616926</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100200.4008016032</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>112688.75366238449</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>113520.26336701101</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>112435.34967393748</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>126534.22750854107</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>140409.99719180007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-57D0-7A43-A393-E696EAE99236}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$I$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>UMAP +IO 80 UFFD Threads</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -847,36 +953,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$G$2:$G$10</c:f>
+              <c:f>data!$O$13:$O$21</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>45514.541896135815</c:v>
+                  <c:v>12331.672668080699</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>76242.756938090883</c:v>
+                  <c:v>17610.28440609316</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>64641.241111829346</c:v>
+                  <c:v>21263.0236019562</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24728.603575756078</c:v>
+                  <c:v>30945.381401825776</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22977.941176470587</c:v>
+                  <c:v>12330.456226880395</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17760.096614925584</c:v>
+                  <c:v>10124.224231318276</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18889.665464024631</c:v>
+                  <c:v>9480.3803528597564</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>17461.148943600489</c:v>
+                  <c:v>9484.6064836769929</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16666.666666666668</c:v>
+                  <c:v>9934.7288315765418</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -884,13 +990,119 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-57D0-7A43-A393-E696EAE99236}"/>
+              <c16:uniqueId val="{00000003-57D0-7A43-A393-E696EAE99236}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$Q$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>UMAP -IO 1 UFFD Thread</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$T$13:$T$21</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$W$2:$W$10</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>34758.428919012862</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64466.21970087674</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60266.377388055203</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60248.222677431018</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>58244.510454889627</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>54917.897742874404</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>49390.03309132217</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>38762.694782541279</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>29145.172102241264</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-57D0-7A43-A393-E696EAE99236}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>data!$I$1</c:f>
@@ -994,15 +1206,15 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
-          <c:order val="2"/>
+          <c:idx val="0"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>data!$I$12</c:f>
+              <c:f>data!$A$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>UMAP +IO 80 UFFD Threads</c:v>
+                  <c:v>NVME DirectIO</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1010,8 +1222,9 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1057,36 +1270,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$O$13:$O$21</c:f>
+              <c:f>data!$G$2:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>12331.672668080699</c:v>
+                  <c:v>45514.541896135815</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17610.28440609316</c:v>
+                  <c:v>76242.756938090883</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21263.0236019562</c:v>
+                  <c:v>64641.241111829346</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30945.381401825776</c:v>
+                  <c:v>24728.603575756078</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12330.456226880395</c:v>
+                  <c:v>22977.941176470587</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10124.224231318276</c:v>
+                  <c:v>17760.096614925584</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9480.3803528597564</c:v>
+                  <c:v>18889.665464024631</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9484.6064836769929</c:v>
+                  <c:v>17461.148943600489</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9934.7288315765418</c:v>
+                  <c:v>16666.666666666668</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1094,217 +1307,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-57D0-7A43-A393-E696EAE99236}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>data!$Q$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>UMAP -IO 1 UFFD Thread</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>data!$T$13:$T$21</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>data!$W$2:$W$10</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>34758.428919012862</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>64466.21970087674</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>60266.377388055203</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>60248.222677431018</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>58244.510454889627</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>54917.897742874404</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>49390.03309132217</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>38762.694782541279</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>29145.172102241264</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-57D0-7A43-A393-E696EAE99236}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>data!$Q$12</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>UMAP -IO 80 UFFD Threads</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>data!$T$13:$T$21</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>data!$W$13:$W$21</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>39384.03371273286</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>52631.57894736842</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>73443.008225616926</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>100200.4008016032</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>112688.75366238449</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>113520.26336701101</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>112435.34967393748</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>126534.22750854107</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>140409.99719180007</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-57D0-7A43-A393-E696EAE99236}"/>
+              <c16:uniqueId val="{00000000-57D0-7A43-A393-E696EAE99236}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1696,15 +1699,15 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="4"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>data!$Y$1</c:f>
+              <c:f>data!$AO$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>NVME DirectIO</c:v>
+                  <c:v>UMAP -IO 80 UFFD Threads</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1712,8 +1715,9 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1759,36 +1763,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$AE$2:$AE$10</c:f>
+              <c:f>data!$AU$13:$AU$21</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>59038.847561695598</c:v>
+                  <c:v>42544.13954477771</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19720.365221163895</c:v>
+                  <c:v>61977.068484660675</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33439.224209998327</c:v>
+                  <c:v>91299.187437231813</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>58606.341206118501</c:v>
+                  <c:v>128139.41568426447</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>39097.626774054814</c:v>
+                  <c:v>149231.45799134456</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>35423.308537017358</c:v>
+                  <c:v>131475.15119642389</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33617.965440731525</c:v>
+                  <c:v>141482.7391058291</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>47136.460051850103</c:v>
+                  <c:v>166472.448809722</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>71700.00717000071</c:v>
+                  <c:v>180082.83810552856</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1796,20 +1800,20 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-077D-944C-BF76-0FF732BF3160}"/>
+              <c16:uniqueId val="{00000004-077D-944C-BF76-0FF732BF3160}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="3"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>data!$AG$1</c:f>
+              <c:f>data!$AG$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>UMAP +IO 1 UFFD Thread</c:v>
+                  <c:v>UMAP +IO 80 UFFD Threads</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1817,8 +1821,9 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1864,36 +1869,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$AM$2:$AM$10</c:f>
+              <c:f>data!$AM$13:$AM$21</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>17472.43723026925</c:v>
+                  <c:v>18903.949034953403</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5972.1459114689087</c:v>
+                  <c:v>10415.256267380459</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5936.3387037410803</c:v>
+                  <c:v>16660.557795474993</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5861.3554970722525</c:v>
+                  <c:v>25859.839668994053</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7030.5194850847529</c:v>
+                  <c:v>32749.304077288358</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7660.1938029032135</c:v>
+                  <c:v>37601.052829479224</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6601.6187169093864</c:v>
+                  <c:v>95219.958103218436</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6374.5019920318728</c:v>
+                  <c:v>125297.58175667209</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7610.3500761035011</c:v>
+                  <c:v>131734.94928204452</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1901,20 +1906,20 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-077D-944C-BF76-0FF732BF3160}"/>
+              <c16:uniqueId val="{00000003-077D-944C-BF76-0FF732BF3160}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
+          <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>data!$AG$12</c:f>
+              <c:f>data!$AO$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>UMAP +IO 80 UFFD Threads</c:v>
+                  <c:v>UMAP -IO 1 UFFD Thread</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1922,8 +1927,9 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
+              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1969,36 +1975,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$AM$13:$AM$21</c:f>
+              <c:f>data!$AU$2:$AU$10</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>18903.949034953403</c:v>
+                  <c:v>49882.775477627576</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10415.256267380459</c:v>
+                  <c:v>62723.452298814525</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16660.557795474993</c:v>
+                  <c:v>74671.445639187572</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25859.839668994053</c:v>
+                  <c:v>78591.637849732782</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32749.304077288358</c:v>
+                  <c:v>73308.408474452022</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37601.052829479224</c:v>
+                  <c:v>70606.509920214638</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>95219.958103218436</c:v>
+                  <c:v>62798.291886460691</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>125297.58175667209</c:v>
+                  <c:v>54525.627044711015</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>131734.94928204452</c:v>
+                  <c:v>43927.081045464533</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2006,20 +2012,20 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-077D-944C-BF76-0FF732BF3160}"/>
+              <c16:uniqueId val="{00000002-077D-944C-BF76-0FF732BF3160}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="1"/>
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>data!$AO$1</c:f>
+              <c:f>data!$AG$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>UMAP -IO 1 UFFD Thread</c:v>
+                  <c:v>UMAP +IO 1 UFFD Thread</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2027,8 +2033,9 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -2074,36 +2081,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$AU$2:$AU$10</c:f>
+              <c:f>data!$AM$2:$AM$10</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>49882.775477627576</c:v>
+                  <c:v>17472.43723026925</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>62723.452298814525</c:v>
+                  <c:v>5972.1459114689087</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>74671.445639187572</c:v>
+                  <c:v>5936.3387037410803</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>78591.637849732782</c:v>
+                  <c:v>5861.3554970722525</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>73308.408474452022</c:v>
+                  <c:v>7030.5194850847529</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>70606.509920214638</c:v>
+                  <c:v>7660.1938029032135</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>62798.291886460691</c:v>
+                  <c:v>6601.6187169093864</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>54525.627044711015</c:v>
+                  <c:v>6374.5019920318728</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43927.081045464533</c:v>
+                  <c:v>7610.3500761035011</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2111,20 +2118,20 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-077D-944C-BF76-0FF732BF3160}"/>
+              <c16:uniqueId val="{00000001-077D-944C-BF76-0FF732BF3160}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="4"/>
+          <c:idx val="0"/>
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>data!$AO$12</c:f>
+              <c:f>data!$Y$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>UMAP -IO 80 UFFD Threads</c:v>
+                  <c:v>NVME DirectIO</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2132,8 +2139,9 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent5"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -2179,36 +2187,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$AU$13:$AU$21</c:f>
+              <c:f>data!$AE$2:$AE$10</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>42544.13954477771</c:v>
+                  <c:v>59038.847561695598</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>61977.068484660675</c:v>
+                  <c:v>19720.365221163895</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>91299.187437231813</c:v>
+                  <c:v>33439.224209998327</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>128139.41568426447</c:v>
+                  <c:v>58606.341206118501</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>149231.45799134456</c:v>
+                  <c:v>39097.626774054814</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>131475.15119642389</c:v>
+                  <c:v>35423.308537017358</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>141482.7391058291</c:v>
+                  <c:v>33617.965440731525</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>166472.448809722</c:v>
+                  <c:v>47136.460051850103</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>180082.83810552856</c:v>
+                  <c:v>71700.00717000071</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2216,7 +2224,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-077D-944C-BF76-0FF732BF3160}"/>
+              <c16:uniqueId val="{00000000-077D-944C-BF76-0FF732BF3160}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3643,7 +3651,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{962B71A9-70A2-094F-942C-93F9CF7B6D6F}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="237" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="234" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3654,7 +3662,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{2BC7DB60-C0F0-A146-96AD-A703487C6965}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="237" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="234" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3665,7 +3673,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8681013" cy="6291055"/>
+    <xdr:ext cx="8678333" cy="6290299"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -3698,7 +3706,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8681013" cy="6291055"/>
+    <xdr:ext cx="8678333" cy="6290299"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">

</xml_diff>